<commit_message>
data uji data latih ganti
</commit_message>
<xml_diff>
--- a/data/1000 twitt data latih pos-neg 50-50.xlsx
+++ b/data/1000 twitt data latih pos-neg 50-50.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\KULIAH\THESIS\PROJECT_SENTIMENMB\Sentiment_merdeka_belajar\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Kuliah\THESIS\PORGRAM_MERDEKA\Sentiment_merdeka_belajar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC5CEC2-0CFD-481B-9BD3-BDC3C0BB7BC0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDB71CB-C7A1-4289-A8DA-6736D5FFB6A1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5605" uniqueCount="3035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5005" uniqueCount="2743">
   <si>
     <t>created</t>
   </si>
@@ -8815,1142 +8815,12 @@
   <si>
     <t>RT @CakKhum: Mas Prabowo malam ini bagus sekali debatnya, menyerang tepat di jantung pertahanan, akhirnya muter jawabannya radar lagi</t>
   </si>
-  <si>
-    <t>Isi pelajarannya dikurangi pak. UN masih gpp.</t>
-  </si>
-  <si>
-    <t>Setuju UN lah, biar kartel kunci UN jg bs makan
-Lapangan kerja meningkat, ekonomi tumbuh</t>
-  </si>
-  <si>
-    <t>Untuk naik level derajat (dan iman) hambaNya.. 
-Allah saja menguji.(QS. Al-Ankabut 2-3)
-Bukan masalah hasil nilai UN nya.
-Proses dalam mendapatkan hasil UN nya sangat penting.. dalam membentuk mental siswa.
-(Kejujuran, kerjakeras, kesabaran ada didalamnya)</t>
-  </si>
-  <si>
-    <t>Y lbh baik UN d'hpz aja..........</t>
-  </si>
-  <si>
-    <t>Nadiem dongggg. Ikutin perkembangan jamannnn</t>
-  </si>
-  <si>
-    <t>masa lalu biarlah jd masa lalu...saatnya yang muda yg berkarya..</t>
-  </si>
-  <si>
-    <t>Jelas #TimNadien lah. Itu Ujian nasional sudah berapa puluh Abad dilakukan? Ada kemajuan ngga pendidikan Indonesia? Cocok ngga tuh UN dengan kebutuhan Industry 4.0 ?</t>
-  </si>
-  <si>
-    <t>Dukung mas Menteri lah..gw yakin dia sangat mengerti apa yg akan dia lakukan dan akan membawa perubahan baru yg positif.</t>
-  </si>
-  <si>
-    <t>Kita doakan saja semoga dapat memberikan dampak positif untuk bangsa ini. yang untuk mewujudkan tujuan Negera mencerdaskan kehidupan bangsa....</t>
-  </si>
-  <si>
-    <t>Kalau bisa via live sama rakyat. Rakyat yang menguji secara akhlak melalui tes pengabdian masyarakat. 
-Ujian tetap dilaksanakan (ulangan harian, semester).
-Kalau bisa ketrampilan kecakapan, penalaran, dan pengamatan diujikan sesuai kebutuhan sekolah.</t>
-  </si>
-  <si>
-    <t>Presiden pasti bisa meroketkan ekonomi Indonesia klo gak ikut Ujian Nasional tapi ikut assessment.</t>
-  </si>
-  <si>
-    <t>Dukung pak mendikbud, UN bkn satu2nya tolak ukur</t>
-  </si>
-  <si>
-    <t>Apresiasi kpd mendikbud hapus un, semestinya th ini (2020) sudah dihapuskan. Kurikulum dasar jg perlu ditinjau lg</t>
-  </si>
-  <si>
-    <t>Hapus lah, manusia tercipta dengan kemampuan berbeda-beda kenapa harus dinilai dengan soal UN yg sama dan  beda urutan nomer saja</t>
-  </si>
-  <si>
-    <t>Nadiem donggg, kalau perlu gausah pake sistem rangking juga, sama waktu sekolahnya jangan kelamaan , maafkan aku mak #anakguru</t>
-  </si>
-  <si>
-    <t>Sebenernya ini wacana dari dulu, kalau memang konsepnya bagus ya why not? Evaluasi? Pasti, gak ada konsep yang perfect</t>
-  </si>
-  <si>
-    <t>Udah bener dana UN mnding buat kegiatan lain utk mempertajam pengetahuan siswa/i. Ga gitu ngefek.</t>
-  </si>
-  <si>
-    <t>Nadiem donk...masa hampir 1 abad gtu aja g ada hasilnya</t>
-  </si>
-  <si>
-    <t>Saya berada di pihak Pak Nadiem. Kenapa? Pak Nadiem tidak sekedar menghapus UN tnpa tujuan melainkan dia pasti memiliki tujuan Salah satunya yaitu siswa Yang berkarakter Dan kreatif :)</t>
-  </si>
-  <si>
-    <t>Menteri ku gak papa biar fokus UTBK</t>
-  </si>
-  <si>
-    <t>Support Nadiem dong....</t>
-  </si>
-  <si>
-    <t>Lembek ketika masih sekolah gak masalah kalau udah di luar sekolah baru masalah, karena siswa punya keahliannya masing-masing</t>
-  </si>
-  <si>
-    <t>Setuju banget, yg lbh penting dia paham sama apa yg diajarkan sehari2 (proses) bukan ngejar nilai akhir alias belajar hanya demi UN tok segala cara ditempuh..</t>
-  </si>
-  <si>
-    <t>Boleh juga un ga jadi syarat kelulusan tp jadi patokan buat dapet sekolah unggulan
-Atau nga nilai un jadi syarat dapet sim kendaraan / pekerjaan   
-Lulus belom pasti sukses itu yang perlu di tanemin buat anak2 muda sekarang</t>
-  </si>
-  <si>
-    <t>Saya percayakan ke Pak Nadiem</t>
-  </si>
-  <si>
-    <t>Setuju dihapus. Kualitas guru, sekolah dan sarpras timpang disana sini tp bobot &amp; kesulitan soal sama...</t>
-  </si>
-  <si>
-    <t>Dukung mas Menteri Nadiem dong. Pak @Pak_JK mah udh generasi jaman baheula..kuno. Perlu gebrakan2 baru.
-#GebrakanNadiem #UjianNasional</t>
-  </si>
-  <si>
-    <t>Duuu sumpa UN tuh ga ngaruh buat masa depn plisss. Klo emng prlu tes utk ukur kmampuan, mnding yg sesuai bkat minat aj. Dripad bljr ipa mtk luamaaaa ngotot bgt cmn buat ujian 3-4 hari, useless si mnurutku, monmaap sbelumnya</t>
-  </si>
-  <si>
-    <t>Setuju UN dihapus</t>
-  </si>
-  <si>
-    <t>Mereka masuk didunia kerja menggunakan skill/keterampilan dalam bidangnya masing- masing bukan dengan angka yang ada di lembar kertas</t>
-  </si>
-  <si>
-    <t>Semoga terwujud. Nda apa ada ujian. Tapi itu bukan penentu kelulusan</t>
-  </si>
-  <si>
-    <t>mending UN dihapus saja, unfaedah!</t>
-  </si>
-  <si>
-    <t>Usul ndan sekolah di hapus saja karena di Indonesia banyak orang pintar, tapi pintarnya di buat membodohi masyarakat. Mending goblok bareng bareng saja biar gak ada penipuan</t>
-  </si>
-  <si>
-    <t>Jujur aja sih, blm ada org sukses sampe sekarang, yg dulu nya enggak pernah ikut ujian , even bill gates ttp ujian pas masuk kuliah meskipun akhirnya enggak kelar</t>
-  </si>
-  <si>
-    <t>Kenapa nggak dihapus dari dulu #peace  @faridaryanidian @fajrimarisa @PatiguRosy</t>
-  </si>
-  <si>
-    <t>Kenapa ga dari duluuuuu yaaa wkwkkw</t>
-  </si>
-  <si>
-    <t>1. Peran aktif guru, anak murid, dan orangtua sangat berpengaruh pada tingkat kepintaran dan pemikiran seorang murid, jgn menilai semua berfokus pada Ujian Nasional yg notabennya hanya tahap sesaat untuk meningkatkan murid ke jenjang pendidikan yg lebih tinggi,</t>
-  </si>
-  <si>
-    <t>2. tetapi dilihat dari proses belajar mwngajar serta peran aktif orangtua akan membuat karakter murid jauh lebih baik, sehingga jika seorang murid tidak memiliki karakter tersebut tetap aja UN tidak UN hasilnya akan sama.</t>
-  </si>
-  <si>
-    <t>saatnya anak2 lebih fokus ke talent yg dia minati dan sukai.. ga terpaku pada les dan les berbagai pelajaran, serta tambahan jam belajar demi kejar hasil UN.. saat kerja nanti ya buat apa</t>
-  </si>
-  <si>
-    <t>Ujian nasional isinya fisika, kimia, matematika, bahasa dll. Siswa terpaku kesana supaya lulus sekolah. Padahal di kuliah ga semua dipakai, di kerja ga semua dipakai. Hilangkan saja UN, jadikan mata pelajaran itu biasa . Biar siswa bisa dr awal fokus ke bidang yg disukai masing2.</t>
-  </si>
-  <si>
-    <t>Penghapusan UN malah bikin para siswa/i hemat uang Pak agar tidak pt pt beli kunci</t>
-  </si>
-  <si>
-    <t>Dan org tuanya jg..ngga perlu ngikutin les sana sini</t>
-  </si>
-  <si>
-    <t>Setuju sih...Tp mohon maaf, saya justru melihat yg takut dievaluasi dan dianggap gagal itu dinas pendidikan setempat, dan  sekolah2....lalu melakukan trik2 yg tdk sehat supaya tetap terlihat bagus. Ini sebenarnya yg harus diperbaiki dulu.</t>
-  </si>
-  <si>
-    <t>kuliah jurusan desain ga ada itu semua hahaha</t>
-  </si>
-  <si>
-    <t>Lembek tidaknya siswa akan terlihat saat masuk dunia kerja, UAN sih ya maapmaap cuma ngelatih skill ngapalin kopean kunci jawaban</t>
-  </si>
-  <si>
-    <t>Khawatir klo UN dihapuskan murid akan menyepelekan proses pembelajaran
-"Toh gak ada UN pasti lulus lah"</t>
-  </si>
-  <si>
-    <t>*begitu ujian nasional ga jadi penentu kelulusan*
-Me ketika jaga ujian di sekolah : *fisika selesei dlm 30 menit, kertas buram msh kosong, ditinggal tidur sama anak2*
-Me : lho ayo soalnya dikerjakan.
-Anak2 : halah, ngga nentuin kelulusan kan bu...
-*</t>
-  </si>
-  <si>
-    <t>Jadi nyepelein gitu ya mba muridnya
-Anak anak emang gitu dikasih enak malah ngelunjak
-Jadi males belajar</t>
-  </si>
-  <si>
-    <t>Tim jangan susahin adekku aja pokoknya soalnya itu pas dia kelas 3smp jangan dijadiin kelinci percobaan doang dia udah berkali2 ganti kurikulum dr kelas 1sd</t>
-  </si>
-  <si>
-    <t>UN tetap wajib diadakan sebagai tolok ukur tingkat keberhasilan proses belajar mengajar NASIONAL.
-Bukan sebagai acuan kelulusan.
-#PertahankanUN</t>
-  </si>
-  <si>
-    <t>misal yang UN di hapus,apa pas SBMPTN mereka ngga kaget ?alhasil,bisa banyak yg ga lolos.
-kalau misal ingin siswa sesuai bakat dan minat,justru perbanyak jumlah SMK drpd SMA.jadi yang tidak terjangkau biaya kuliah,punya keterampilan yang dimiliki setelah lulus.</t>
-  </si>
-  <si>
-    <t>JK juga lembek selama jdi Wapres kemarin, Cuman meng aamiini Jokowi Aja</t>
-  </si>
-  <si>
-    <t>Anda yg Who? 
-Masih mau ikut UN? Hahahaha 
-Ujian Ndungu..</t>
-  </si>
-  <si>
-    <t>@Kemdikbud_RI @KSPgoid Menjadi lembek apanya? JK kan bagian dari "old fashion" apa yg sdh dia jalankan dulu hrsnya tetap jalan tanpa perlu updated data dan apalagi eco system sosial jaman now. Jd tak perlu dibahas omongan JK.</t>
-  </si>
-  <si>
-    <t>Ujian Nyontek (UN) haduh uda tau sama tau .</t>
-  </si>
-  <si>
-    <t>Kenapa ga dari dulu pak ,kenapa gak pas saya masih sekula:(</t>
-  </si>
-  <si>
-    <t>Sekalian gak usah sekolah aja, biar jadi driver ojol semua lulusan smu smk</t>
-  </si>
-  <si>
-    <t>Skripsi sekalian pak
-Tahun ini kalo perlu, biar saia langsung lulus, karena skripsian buang-buang banyak kertas pak</t>
-  </si>
-  <si>
-    <t>UAN itu sejati nya membuat siswa menjadi kompak dalam satu minggu. misalnya kompak patungan beli kunci jawaban, dan kompak sharing jawaban</t>
-  </si>
-  <si>
-    <t>Yaaelaah JK... Ente dah ngga masuk lagi jaman yg skarang... Pendidikan dulu beda dgn yg skarang.... Sudah laah JK mending ngemong cucu yeee....
-Biar urusan UN dah ada yg ngurus... 
-Gitu yeee...</t>
-  </si>
-  <si>
-    <t>Jngn di hapus biar penerus bisa merasakan begitu sulinya UN</t>
-  </si>
-  <si>
-    <t>Sy orang yg tdk stuju dg dihapuskannya UN. Krna sy mrasa sistem disni blum siap dg sistem pnilaian brbasis ktrampilan, krn nanti yg mngukur bgus/tdak nya adl gru, klo SDM, Infrastruktur, pemerataan pendidikan sdh trjadu, bru sya stuju dgn sistem ini @Kemdikbud_RI @Itjen_Kemdikbud</t>
-  </si>
-  <si>
-    <t>UN dihapus = Pendidikan mundur 100th., apa masalahnya dg UN?, masalahnya dicarikan solusi, bukan UN dhps.</t>
-  </si>
-  <si>
-    <t>JK otaknya dah gak update, pentium 1 diadu dgn core i5 ya jauuh kececer.</t>
-  </si>
-  <si>
-    <t>Apakah UN terkait dengan lapangan kerja... ??!,
-Yg jelas UN pernah tercatat sbg penyebab Siswa stress dan ato Tindak Bunuh Diri.
-Bekerjalah yg BETTER broo Nadiem sesuai VisiMisi Presiden @jokowi, bukan yg lain !!
-#GoToRank20</t>
-  </si>
-  <si>
-    <t>Makin bikin ruwet para siswa &amp; orang tua.. ganti-ganti kebijakan terus.. bikin siswa jadi males buat belajar.. kemaren sistem zonasi.. sekarang UN dihapus.. next.. apalagi boss</t>
-  </si>
-  <si>
-    <t>Harus ada penggantinya pak. Hasil UN itu kadang kala juga buat melihat proses pembelajaran di suatu sekolah, dan itu jadi penilaian untuk sekolah secara umum.
-Apalagi investasi di bidang CBT untuk UNBK sdh besar, sayang kalau nganggur lagi.....</t>
-  </si>
-  <si>
-    <t>KPAI dukung sistem zonasi PPDB https://gresikmenulis.com/blog/kpai-dukung-sistem-zonasi-ppdb/ …</t>
-  </si>
-  <si>
-    <t>#KAMUHARUSTAU Zonasi dalam PPDB diyakini mendorong terciptanya pendidikan keadilan bagi anak-anak Indonesia sebagaimana diamanatkan dalam konstitusi Republik Indonesia. #ZonasiSekolah #PPDB</t>
-  </si>
-  <si>
-    <t>Dalam penerimaan peserta didik baru (PPDB), Kemendikbud tetap menggunakan sistem zonasi dengan kebijakan yang lebih fleksibel untuk mengakomodasi ketimpangan akses dan kualitas di berbagai daerah. #IndonesiaMerdekaBelajar #MerdekaBelajar</t>
-  </si>
-  <si>
-    <t>KPAI dukung sistem zonasi PPDB https://www.antaranews.com/video/1201471/kpai-dukung-sistem-zonasi-ppdb …</t>
-  </si>
-  <si>
-    <t>#MasMenteri menyampaikan bahwa dalam Penerimaan Peserta Didik Baru (PPDB) Tahun 2020 mendatang @Kemdikbud_RI tetap menggunakan sistem zonasi dgn kebijakan yang lebih fleksibel untuk mengakomodasi ketimpangan akses dan kualitas di berbagai daerah. #MerdekaBelajar</t>
-  </si>
-  <si>
-    <t>Jalur prestasi lebih banyak lagi kuotanya ini.. Dari 15 ke 30 persen... Cocok buat anakku yang punya keahlian di luar bidang akademik</t>
-  </si>
-  <si>
-    <t>Mas Menteri mengumumkan tahun 2020, USBN diganti dengan ujian asesmen yang diselenggarakan hanya oleh sekolah. Ujian kompetensi siswa bisa dalam bentuk tertulis dan/atau bentuk lain seperti portofolio dan penugasan. Dengan begitu, guru dan sekolah lebih merdeka. #MerdekaBelajar</t>
-  </si>
-  <si>
-    <t>Kenapa sih adik-adik ku risau dengan sistem zonasi. Kayak gak PD sama kemapuan sendiri... Padahal kalau kalian bisa dapet nilai rata rata diatas 9 harusnya PD bakal bisa struggle di sekolah yg katanya tidak favorit... #UnpopularOpinion #Zonasi #PPDB</t>
-  </si>
-  <si>
-    <t>Yg punya konsep hapus sistem #zonasi #ppdb itu yg layak didukung Cc @jokowi</t>
-  </si>
-  <si>
-    <t>Alhamdulillahirabilalaminnnn!! Yeay Banzaai! Akhirnya harapan gw terwujudkan oleh Pemerintah Pendidikan sekarang! ZONASI itu penting, kesamarataan pendidikan juga harus ditingkatkan. #Zonasi #PPDB</t>
-  </si>
-  <si>
-    <t>Mendikbud menyampaikan bahwa dalam Penerimaan Peserta  Didik Baru (PPDB) Tahun 2020 mendatang Kemendikbud tetap menggunakan sistem zonasi dengan kebijakan yang lebih fleksibel untuk mengakomodasi ketimpangan akses dan kualitas di berbagai daerah. 
-#MerdekaBelajar</t>
-  </si>
-  <si>
-    <t>Tak Hanya Hapus UN, Pendidikan Era Nadiem Makarim Juga Bakal Ubah Sistem Zonasi PPDB http://dlvr.it/RL6k80 pic.twitter.com/I7WNIoZn4L</t>
-  </si>
-  <si>
-    <t>Lagi rame #PPDBZonasi yah? sudah pada paham belum apasih sistem zonasi itu? #PPDB #Zonasi</t>
-  </si>
-  <si>
-    <t>Min di ig zonasi 90% mohon untuk di ralat🙏🙏</t>
-  </si>
-  <si>
-    <t>Di sistem zonasi baru, jalur perpindahan ada 5%. Kalau tidak diberikan aturan khusus, amat sangat mungkin bagi oknum (kepsek) sekolah melakukan praktek suap mas menteri. Anda yakin bisa mencegah praktek suap mas menteri?</t>
-  </si>
-  <si>
-    <t>bagaimana dengan zonasi apakah bisa di nilai berhasil???</t>
-  </si>
-  <si>
-    <t>Tolong zonasi kepala sekolah bisa dilihat dari KTP nya bukan wilayah kabupaten di mana sekolah itu sangat jauh dari sekolah yang dipimpinnya sebab sekolah kami amburadul karenanya.</t>
-  </si>
-  <si>
-    <t>Zonasi dihapusin aja pak..bikin pusing orang tua..n susah murid, itu mendikbud yg sblumnya bikin susah orang tua murid mas mentri jd dihapus aja zonasi jd ky dulu ngk bikin susah orang tua murid</t>
-  </si>
-  <si>
-    <t>SETUJU PAK, kalau bisa SEPERTI DULU yaitu SP plus GBPP. ZONASI diHAPUS.</t>
-  </si>
-  <si>
-    <t>"ZONASI" adalah PRESTASI=KALAH DENGAN GOOGLE MAP</t>
-  </si>
-  <si>
-    <t>Mendikbud Nadiem Makarim mengubah jalur zonasi PPDB alias penerimaan peserta didik baru, menjadi minimum 50 persen. #PPDBsistemzonasihttp://m.jpnn.com/news/kpai-soroti-kebijakan-nadiem-makarim-ubah-persentase-zonasi-ppdb …</t>
-  </si>
-  <si>
-    <t>PPDB 2020 Tetap Sistem Zonasi, Kuota Jalur Prestasi Ditambah The post  https://www.liputan.co.id/2019/12/ppdb-2020-tetap-sistem-zonasi-kuota-jalur-prestasi-ditambah/ …</t>
-  </si>
-  <si>
-    <t>Sistem Zonasi PPDB, Bandung Lebih Dulu https://www.dara.co.id/sistem-zonasi-ppdb-bandung-lebih-dulu.html …pic.twitter.com/ne4uTRP3ih</t>
-  </si>
-  <si>
-    <t>PPDB 2020 tetap gunakan sistem Zonasi, jatah jalur prestasi naik
-#KomisiAndaElshintapic.twitter.com/9RU0sE7I4q</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sistem zonasi PPDB direvisi, 30 persen dari jalur prestasi </t>
-  </si>
-  <si>
-    <t>Komposisi Kuota PPDB Zonasi 2020 Dirubah
-https://www.radarpena.id/nasional/2019/12/13/komposisi-kuota-ppdb-zonasi-2020-dirubah/ …pic.twitter.com/xPcgKjnBpG</t>
-  </si>
-  <si>
-    <t>Nadiem Ubah Proporsi PPDB Sistem Zonasi, Kuota Jalur Prestasi Jadi 30 Persen http://dlvr.it/RL3vHV pic.twitter.com/Vk7pp8bdZb</t>
-  </si>
-  <si>
-    <t>Kuota Zonasi di PPDB Turun Jadi 50 Persen https://andalannews.com/kuota-zonasi-di-ppdb-turun-jadi-50-persen/21073/ …pic.twitter.com/xLUgMQRQVv</t>
-  </si>
-  <si>
-    <t>Peraturan Penerimaan Peserta Didik (PPDB) Zonasi,
-#MerdekaBelajar pic.twitter.com/FS9Ki2QY0W</t>
-  </si>
-  <si>
-    <t>Nadiem tengah menyiapkan 4 rencana kebijakan pendidikan yg disebutnya dgn kebijakan“Merdeka Belajar” itu. Kebijakan perubahan pd USBN, Ujian Nasional (UN), Rencana Pelaksanaan Pembelajaran (RPP), dan Peraturan Penerimaan Peserta Didik Baru (PPDB) Zonasi.</t>
-  </si>
-  <si>
-    <t>Kali ini di FGD IPNU DKI Jakarta membahas tentang PPDB dengan sistem ZONASI apakah efektif atau tidak ? #nahdlatululama #nu #ipnu #fgd #zonasi #ppdb #ppdbzonasi</t>
-  </si>
-  <si>
-    <t>FSGI Apresiasi Gugatan MA Tolak Uji Materi Zonasi PPDB https://tribunasia.com/index.php/2019/12/11/fsgi-apresiasi-gugatan-ma-tolak-uji-materi-zonasi-ppdb/ …pic.twitter.com/r8UHwvnQau</t>
-  </si>
-  <si>
-    <t>Gara2 zonasi ppdb kmrin,anakku g ktrima di sekolah negeri..yg pelosok2 dulu pak dibngun kenapa di kecamatan kami g ada sma negeri..cma ada 1 sma negeri hrs bersaing dgn kec2.lain..yg diterima yg deket2 sekolah saja..miris..</t>
-  </si>
-  <si>
-    <t>#Kom10 Rano Karno 
-@PDI_Perjuangan
-#Banten3 : masalah zonasi di tangsel masih adanya pungli dalam PPDB jadi tidak usah jauh-jauh ke daerah.</t>
-  </si>
-  <si>
-    <t>Kalau melihat ini, Porsi Zonasi dlm PPDB kok malah dikurangi ya @Kemdikbud_RI</t>
-  </si>
-  <si>
-    <t>Skala Prioritas aja,Opsinya PPDB dihapus atau mau yang UN dijahapus.Jika melihat banyaknya kecurangan di PPDB Jalur Zonasi Setiap tahun,sebaiknya UN jangan dihapus.Saran Saya sebaiknya kembalikan PPDB ke Sistem lama dimana nilai UN dijadikan kualifikasi untuk diterima di Sekolah!</t>
-  </si>
-  <si>
-    <t>Ada 95 Aduan Terkait Zonasi PPDB, KPAI Minta Pemerintah Tambah SMP-SMAN https://mandrigunawanberita.wordpress.com/2019/12/09/ada-95-aduan-terkait-zonasi-ppdb-kpai-minta-pemerintah-tambah-smp-sman/ …</t>
-  </si>
-  <si>
-    <t>Seharusnya UN dihapuskan saja dari agenda pendidikan Indonesia karena tidak lagi relevan, apalagi dengan adanya sistem zonasi Penerimaan Peserta Didik Badu (PPDB) yang mulai tahun 2018 kemarin dilaksanakan serentak dan membuat gejolak di masyarakat. Ubaid Matraji, #UjianNasional pic.twitter.com/A82LaGPhUG</t>
-  </si>
-  <si>
-    <t>Trus w tiba tiba kepikiran: gimana kalo misalkan Nadiem Makarim ngubah peraturan PPDB 2020 jadi ga ada zonasi lagi trus masuk SMA negeri pake nilai UN? WOKWOWKWOWKOWKW AUTO MAMPUS SIA ANYING, batinku dalam hati.</t>
-  </si>
-  <si>
-    <t>Bila TDK ada UN, standard apa yg di pakai untuk PPDB??? Zonasi TDK menjawab masalah pendidikan dasar.</t>
-  </si>
-  <si>
-    <t>2018: kelinci percobaan unbk dan kelinci percobaan ppdb sistem zonasi
-2021: kelinci percobaan asesmen kompetensi mininum dan survei karakter
-(apaan lg si astaga puyeng jd percobaan trs) https://twitter.com/collegemenfess/status/1204609503267717120 …</t>
-  </si>
-  <si>
-    <t>KPAI Kritik Pengurangan Kuota Jalur Zonasi PPDB http://bit.ly/2PGK85i</t>
-  </si>
-  <si>
-    <t>Zonasi di era Menteri Nadiem kemunduran karena diturunkan drastis menjadi 50 persen. http://republika.co.id/berita/pendidikan/eduaction/19/12/12/q2e0x7428-kpai-kritisi-pengurangan-jumlah-persentase-ppdb-zonasi-murni …</t>
-  </si>
-  <si>
-    <t>Logika guru ini terbolak-balik, kalo kepengen anak-anak sekolahmu nilainya tinggi ya bikin pinter anak2 didikmu, bukan melarang anak didik orang lain pinter....hadeuuuuuhhhhhttps://m.kumparan.com/kumparannews/federasi-guru-khawatir-nadiem-hentikan-ppdb-sistem-zonasi-1sPxfzZ3ucz?ref=register …</t>
-  </si>
-  <si>
-    <t>Anggota DPR sebut salah satu kekurangan PPDB Zonasi adalah di wilayah perbatasan http://republika.co.id/berita/nasional/umum/19/12/10/q2aovw349-anggota-dpr-sistem-zonasi-masih-relavan …</t>
-  </si>
-  <si>
-    <t>Dgn sistem zonasi kita tdk lagi melihat "sekolah yang bagus" 
-https://news.detik.com/berita/d-4591338/mendikbud-paparkan-kelebihan-sistem-zonasi-di-ppdb …</t>
-  </si>
-  <si>
-    <t>"Merdeka Belajar" saya masih bias dari filosofi Kemdikbud era Jokowi jilid 2. Ada empat pilar; USBN, UN, RPP, dan Zonasi. Letak yang dicetus sebagai Merdeka Belajar ada di pilar keberapa? USBN konsepnya KTI, UN dilakukan di kelas XI, dan Zonasi PPDB. #merdekabelajar</t>
-  </si>
-  <si>
-    <t>KPAI Terima 95 Pengaduan Terkait Zonasi PPDB https://www.validnews.id/-KPAI-Terima-95-Pengaduan-Terkait-Zonasi-PPDB--Sfn …</t>
-  </si>
-  <si>
-    <t>#TOPNEWS Pukul 14.00 WIB 
-Ada 95 Aduan Terkait Zonasi PPDB, KPAI Minta Pemerintah Tambah SMP-SMAN</t>
-  </si>
-  <si>
-    <t>aduh mudah2 tahun 2020 dan kelanjutanya tdk ada lagi sistem Zonasi krn kasihan anak2 yg prestasi sangat susah cari sekolah jika rmhnya tdk dpt jatah sekolah yg dekat dngn rmh. Masa harus masuk Swasta kl ada dana kl tdk... Apa tdk sekolah. beli kursi aja mahal bngt.</t>
-  </si>
-  <si>
-    <t>Yng saya tahu sistem zonasi, menjadikan orang tua memalsukan kartu keluarga demi masuk sek tsbt</t>
-  </si>
-  <si>
-    <t>mbalik lagi uber2an sekolah favorit</t>
-  </si>
-  <si>
-    <t>yaiyalah. kondisi saat ini aja anak2 yg nilainya bagus tapi rumahnya jauh dari sekolah yang bagus, jadi harus kalah sama anak2 yg nilainya kurang bagus karena mereka rumahnya lebih dekat dgn sekolah tsb.</t>
-  </si>
-  <si>
-    <t>Replying to @ohdeartegar @Outstandjing Masih ada "kelas" antara sekolah kita, secara kualitas memang belum merata. Zonasi ini memaksa semua sekolah buat sama" jadi sekolah favorit/berkualitas tpi itulah kata mas mentri prosesnya ga dibarengi sama peningkatan kualitas sekolah.</t>
-  </si>
-  <si>
-    <t>Bukanya salah satu tujuan zonasi itu pemerataan pendidikan sehingga tidak ada satu sekolah yang isi nya semua pandai dan sekolah lainya tidak begitu pandai? Dengan meratanya sdm, tidak ada siswa yang tidak bisa belajar dari temannya</t>
-  </si>
-  <si>
-    <t>Gak relevan kalo dikaitkan dengan nilai bagus krn kebijakannya ke depan gk bakalan berorientasi ke nilai. Buktinya proporsi jatah siswa ditambah buat jalur afirmasi bukan nambah jalur prestasi. Jd semangat pemerataan mutu pendidikan sih bakal tetap ada.</t>
-  </si>
-  <si>
-    <t>paham ini mungkin maksudnya lebih ke "penyamarataan kualitas" jadi gaada sekolah yg dinilai bagus atau jelek karna bagus semua. tapi kenyaataannya yg terjadi malah penurunan kualitas kalo dilihat scr output dari nilai un yg menurun karena sistem zonasi yg terlalu banyak</t>
-  </si>
-  <si>
-    <t>wkwk iya bener, kadang suka mikir ktanya zonasi ko masih bnyk yg telat</t>
-  </si>
-  <si>
-    <t>Sistem zonasi maksudnya baik, cuma belum siap dilakukan karena pemerataan sekolah belum mumpuni. Mungkin nanti saat minima satu smp sma sudah tersedia tiap satu kecamatan.</t>
-  </si>
-  <si>
-    <t>Anak berburu sekolah yang favorit. Padahal sekolah favorit itu bersumber dari kreatifitas gurunya. Akan lebih baik kalau guru yg kreatif tersebut disebar ke banyak sekolah lain untuk meningkatkan kualitas sekolah "biasa" menjadi sekolah "favorit".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kalo mau mengadu kemana? Dulu pemerimaan ikut zonasi sekarang klas 2 sekolahnya pindah keluar zonasi. Tambah jauh lagi </t>
-  </si>
-  <si>
-    <t>Masalahnya jalur jalur yg loe bikin bisa dibeli harga mulai dr 2 jt an</t>
-  </si>
-  <si>
-    <t>"PPDB dengan sistem zonasi tidak akan terjadi masalah jika kondisi dan kualitas pendidikan di Indonesia sudah relatif sama. Baik dari kualitas guru maupun sarana prasana," #zonasi #ppdb</t>
-  </si>
-  <si>
-    <t>Jadi korban PPDB Zonasi, puluhan orangtua dan siswa demo di Depok. #iNews #iNewsMalam #Zonasi #PPDB #Pendidikan #Demo #Depok</t>
-  </si>
-  <si>
-    <t>Kisruh penerimaan peserta didik baru atau PPDB tak kunjung usai. Orang tua murid di SMA Negeri 9 Tangerang protes karena persyaratan wajib memiliki Kartu Indonesia Sehat (KIS) saat pendaftaran. #penerimaansiswa #ppdb #zonasi #Tangerang #iNewsSiang #iNews</t>
-  </si>
-  <si>
-    <t>Pesimis melihat masa depan smansa bogor akibat zonasi setelah melihat data pendaftar di website PPDB #ZONASI #ppdb</t>
-  </si>
-  <si>
-    <t>Sekali lagi problemnya bukan favorit atau non-favorit, tapi kurangnya kapasitas. Jawaban pemerintah selalu orientasi jangka menengah/panjang. Lha anak2 pintêr yang SEKARANG tidak kebagian sekolah ini bagaimana? #ppdb #ppdb2019 #zonasi</t>
-  </si>
-  <si>
-    <t>Ditulis dan disuarakan oleh : @alwin_jalliyani . Selamat menikmati hidangan musikalisasi, curahan hati pelajar mengenai sistem zonasi. Semoga mudah dimengerti.</t>
-  </si>
-  <si>
-    <t>Metode PPDB sll jadi perbincangan hangat. Memasuki tapel 2019/2020 ini banyak keluhan di berbagai daerah. Presiden Jokowi akan mengevaluasi Zonasi PPDB. Smg hasilnya bermanfaat tanpa menimbulkan gejolak bg masyarakat. #zonasi #ppdb #zonasippdb #pendidikanindonesia #evaluasippdb</t>
-  </si>
-  <si>
-    <t>Iya juga sih. Ngapain sekolah ke luar negeri ? Kalau kuliah wajar sih. Kalau ortunya tiba2 pindah tugas keluar negeri dan anaknya wajib ikut. Masak anaknya gak bisa sekolah ikut bapaknya disana ? #zonasisekolah #zonasi #ppdb</t>
-  </si>
-  <si>
-    <t>Buat apa nilai UN tinggi terus pinternya naudzubillah, kalo jarak dari sekolah tujuan jauh #PPDB2019 #PPDB #PPDBjatim #ZONASI</t>
-  </si>
-  <si>
-    <t>Aku cukup bersyukur melampaui semua proses termasuk di bangku sekolah tidak favorit. Mengenal orang2 hebat di lingkungan ini, dan ntah apa jadinya kalau aku berproses melalui kanal lain. #zonasi #PPDB</t>
-  </si>
-  <si>
-    <t>Apa para orang tua tidak percaya Tuhan? Sehingga hanya mengandalkan sekolah yg dianggap favorit utk menuju kesuksesan? #zonasi #PPDB</t>
-  </si>
-  <si>
-    <t>#zonasi #ppdb akan memakan korban. Siswa/i berprestasi -nem tinggi - bakalan gak dapet sekolah walaupun di zona sendiri...</t>
-  </si>
-  <si>
-    <t>4. Fleksibelitas zonasi PPDB. Mendikbud memperbaiki kuota PPDB tahun lalu yang cukup ekstrem dan kacau.</t>
-  </si>
-  <si>
-    <t>3. Penyederhanaan RPP (Rencana Pelaksanaan Pembelajaran)
-RPP yang awalnya berisi 13 komponen disederhanakan menjadi 3: tujuan, kegiatan, dan penilaian. Agar guru tidak terbebani dgn urusan administrasi &amp; dapat berfokus pada pengaplikasian serta evaluasi pembelajaran yg dibuat.</t>
-  </si>
-  <si>
-    <t>1 halaman saja cukup!
-Yang pernah buat RPP pasti tau rasanya gmna hahaha https://www.profesiguru.org/2019/12/komponen-inti-format-rpp-terbaru-dari-nadiem.html …</t>
-  </si>
-  <si>
-    <t>walaupun bukan anak pendidikan, tp si mas yg anak pendidikan selalu ngedumel tiap penyusunan RPP. Begitu jg si tante yg skrg jd guru SD. 
-Alhamdulillah kalo masalah RPP jd lebih disederhanakan. https://twitter.com/sheggario/status/1204681151710777344 …</t>
-  </si>
-  <si>
-    <t>RPP ughh jd inget bikin RPP segambreng2. Blm apa2 udh nyeri pinggang duduk mulu ngetik dpn komputer. Blm ngajar dan nyiapin bhn ajar. Makanya gw bilang jd guru itu capek. Bukan capek ngajar, tp tetek bengeknya bnyk. Alhamdulillah akan disederhanakan. https://twitter.com/sheggario/status/1204681151710777344 …</t>
-  </si>
-  <si>
-    <t>Trending Topik Guru Saat ini RPP 1 Lembar
-yang telah disederhanakan oleh Kemdikbud. 
-Berikut contoh RPP 1 Lembar
-Kredit : @hernibudiati (Facebook)</t>
-  </si>
-  <si>
-    <t>Format RPP Terbaru yang disederhanakan Mendikbud Nadiem "Merdeka Belajar" dalam Prakteknya Guru secara bebas dapat memilih, membuat, menggunakan, dan mengembangkan Format RPP Terbaru.
-Penulisan RPP dilakukan dengan efisien dan efe…https://lnkd.in/fNGvuxn  https://lnkd.in/fh6_KVX</t>
-  </si>
-  <si>
-    <t>Rpp awalnya 13 komponen disederhanakan jadi 1 lembar, makasi bapak 
-Pak, ini buku kerja 1-4 apa bisa disederhanakan juga  pic.twitter.com/A9O09LherW</t>
-  </si>
-  <si>
-    <t>RPP DISEDERHANAKAN ?
-PUJITUHANNN 
-WOI GUA BAHAGIA GA PERLU SUSAH2 BIKIN RPP DISETIAP KD WOYYYY</t>
-  </si>
-  <si>
-    <t>Lagiii nih.. Mendikbud Nadiem Makarim juga mengumumkan rencana pelaksana pembelajaran (RPP) akan disederhanakan. 
-#GebrakanNadiem #MerdekaBelajar pic.twitter.com/CYEqoi5BZq</t>
-  </si>
-  <si>
-    <t>#Kom10 Syaiful Huda 
-@FraksiPKB
-#Jabar7 : Kami setuju dengan RPP disederhanakan menjadi 1 lembaga, kami meminta mendapatkan jaminan untuk guru tidak menjadi malas untuk memberikan materi untuk mendidik.</t>
-  </si>
-  <si>
-    <t>Guru saat ini lebih direpotkan membuat laporan dibanding mengajar murid2 di kelas. Utk itu jika RPP disederhanakan diharapkan dpt mengurangi beban guru dan mengembalikan fokus ke pembelajaran di kelas</t>
-  </si>
-  <si>
-    <t>Penyusunan Rencana Pelaksanaan Pembelajaran (RPP) akan disederhanakan jadi 1 hlmn. Guru dpt bebas memilih, membuat, menggunakan, &amp; mengembangkan format RPP. 3 komponen inti RPP yaitu tujuan pembelajaran, kegiatan pembelajaran, &amp; asesmen. #MerdekaBelajar
-#Edutore #SemuaBisaPintar</t>
-  </si>
-  <si>
-    <t>#MerdekaBelajar #RPPdisederhanakan #DesainPengajaranMerdekaBelajar pic.twitter.com/ib9JJRdLEs</t>
-  </si>
-  <si>
-    <t>#MerdekaBelajar #IndonesiaMerdekaBelajar bukan cuma untuk siswa/siswi dan menghilangkan kecemasan kelusrga . Tapi juga untuk PARA GURU. Rencana Pelaksanaan Pembelajaran (RPP) yang disusun guru akan disederhanakan.</t>
-  </si>
-  <si>
-    <t>@WikiDPR #Kom10 Syaiful Huda @FraksiPKB #Jabar7 : Kami setuju dengan RPP disederhanakan menjadi 1 lembaga, kami meminta mendapatkan jaminan untuk guru tidak menjadi malas untuk memberikan materi untuk mendidik.</t>
-  </si>
-  <si>
-    <t>Kami btuh buku yg bagus pak. Buku yg menuangkan seluruh hrapan kuriklum qt. 
-RPP dapat disederhanakan jika buku siswa dan buku guru yg memuat seluruh aktiVtas bljar yg diharapkan .
-Mantapkan buku untuk pembelajaran yg bermutu. 
-GOOD LUCK PAK MENTRI,kami berharap bnyak kpd Bapak.</t>
-  </si>
-  <si>
-    <t>Selama ini, guru waktunya sering terbuang untuk Rencana Pelaksanaan Pembelajaran (RPP). Padahal, jika bisa disederhanakan akan lebih efektif. http://dlvr.it/RK3Zrp</t>
-  </si>
-  <si>
-    <t>5. Seluruh beban administrasi Guru dibuat online dan disederhanakan, RPP cukup 1-2 halaman tapi jelas tujuan
-Aplikasi pembelajaran tdk lagi berkas administrasi dlm bentuk “hard copy”, verifikasi keaslian dilakukan secara acak dgn kewajiban menunjukkan
-berkas asli, bukan Foto Copy</t>
-  </si>
-  <si>
-    <t>dan ada kecenderungan saya utk melakukan pengulangan bagian2 RPP, mungkin bisa disederhanakan pembuatannya, menjadi...</t>
-  </si>
-  <si>
-    <t>Selama ini, guru waktunya sering terbuang untuk Rencana Pelaksanaan Pembelajaran (RPP). Padahal, jika bisa disederhanakan akan lebih efektif. http://dlvr.it/RK3bMx</t>
-  </si>
-  <si>
-    <t>5. Seluruh beban administrasi guru dibuat dlm online &amp; lebih disederhanakan, RPP cukup 1-2 halmn tp jelas tujuan dan aplikasi pbelajarannya, tak lg berkas administrasi dlm bentuk “hard copy”, verifikasi keaslian dilakukan acak dg kewajiban menunjukkan berkas asli, bukan FC</t>
-  </si>
-  <si>
-    <t>5. Seluruh beban administrasi guru dibuat DALAM JARINGAN (ONLINE) dan lebih disederhanakan, RPP cukup 1-2 halaman tapi jelas tujuan dan aplikasi pembelajarannya, tak ada lagi berkas administrasi dalam bentuk “hard copy”..</t>
-  </si>
-  <si>
-    <t>@RPP_Aomine dapat menumbuhkan minat di dalam diri sendiri. Ya, bisa disederhanakan; dia datang, setelah itu dapat imbalan istimewa.</t>
-  </si>
-  <si>
-    <t>5). Seluruh beban administrasi guru dibuat dalam jaringan (online) dan lebih disederhanakan, RPP cukup 1-2 halaman tapi jelas tujuan dan aplikasi pembelajarannya, tak ada lagi berkas administrasi dalam bentuk “hard copy”,</t>
-  </si>
-  <si>
-    <t>Replying to @sheggario Alhamdulillah gw kagak perlu ngitungin salam berapa menit kedalam RPP lagi</t>
-  </si>
-  <si>
-    <t>3. Pemangkasan Rencana Pelaksanaan Pembelajaran. RPP akan dibuat sesimpel mungkin sehingga guru akan lebih fokus mendesain pengembangan siswa. Langkah bagus memotong birokrasi yang terbelit-belit.</t>
-  </si>
-  <si>
-    <t>Alhamdulillah,semoga segera di singkronkan jg dg indikator pemenuhan akriditasi dan Rapot PMP yg terkait poin utk RPP. karna jika tidak tetap saja kami para guru harus membuat RPP yg sesuai dg indikator yg diminta, demi memenuhi kriteria akriditasi dan rapot PMP sekolah. Alhamdulillah,semoga segera di singkronkan jg dg indikator pemenuhan akriditasi dan Rapot PMP yg terkait poin utk RPP. karna jika tidak tetap saja kami para guru harus membuat RPP yg sesuai dg indikator yg diminta, demi memenuhi kriteria akriditasi dan rapot PMP sekolah.</t>
-  </si>
-  <si>
-    <t>Rayu Anika iya bu,,blm lagi komponen di Akreditasi sekolah,,utk misalnya poin sesederhana Hand out sj harus A,B,C,D syaratnya😬
-dan mudah2 ini segera benar2 disingkronkan oleh bapak menteri kita,
-Sehingga merdeka belajar benar2 terwujud🥰💪💪</t>
-  </si>
-  <si>
-    <r>
-      <t>semoga terus dpt dibenahi y ibu....oleh bpk menteri kita</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>🥰🥰</t>
-    </r>
-  </si>
-  <si>
-    <t>Coba pak mentri setelah segalanya disederhanakan tolong pak perhatikan guru honor yg sudah lama mengabdi tapi masih belum lulus di tes cpns prioritaskan pak utk pengangkatannya trimakasih</t>
-  </si>
-  <si>
-    <t>Alhamdulillah mudah mudahan guru tidak di beratkan oleh administrasi terus biar ,,bisa fokus membimbing,,mengarahkan dan mengajarkan ,tolong juga diperhatikan kesejahteraan kaum guru honorer supaya lebih semangat untuk menunjang kehidupannya,</t>
-  </si>
-  <si>
-    <t>Alhamdulillah smg rencana Pak menteri yg baru ini bs membuat pendidikan Indonesia tambah maju....</t>
-  </si>
-  <si>
-    <r>
-      <t>Smg ini bertahap satu persatu dimulai dr pekerjaan guru yg dipermudah setelah itu baru tunjangan/honor guru sesuai UMK dan dibyrkan perbulan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>🤔</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">alhamdulillah..ini adalah keputusan </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDB831C"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>terbaik</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> yang dilakukan Mas Menteri...terimakasih telah memerdekakan guru...</t>
-    </r>
-  </si>
-  <si>
-    <t>Terimakasih pak...
-Semoga disederhanakan juga urusan kenaikan pangkat guru ya pak...</t>
-  </si>
-  <si>
-    <t>Alhamdulillah..
-ditunggu realisasinya pa, mudah2 bisa scepatnya.</t>
-  </si>
-  <si>
-    <t>Tujuan, kegiatannya dan penilaian.
-Yg ditulis sedikit, yg perlu tingkatkan adalah kerjanya.</t>
-  </si>
-  <si>
-    <t>Setuju jd lebih jd lebih efektif dan efesien, ringkas dan jelas.
-Semoga begitu jg dg format peniliaannya. Jgn membuat format yg bertele2 utk memperoleh hasil angka/nilai untuk anak.</t>
-  </si>
-  <si>
-    <t>Saya suka jika tugas guru menjadi Ringan... Tetapi kualitas tetap harus dipertahankan</t>
-  </si>
-  <si>
-    <t>Semoga bisa meringankan beban para operator</t>
-  </si>
-  <si>
-    <t>Oklah, semoga rencana bukan sekedar rencana dan membawa dampak baik bagi indonesia #GebrakanNadiem</t>
-  </si>
-  <si>
-    <t>Komponen Inti Format RPP Terbaru yang disederhanakan Mendikbud Nadiem "Merdeka Belajar" https://www.profesiguru.org/2019/12/komponen-inti-format-rpp-terbaru-dari-nadiem.html …</t>
-  </si>
-  <si>
-    <t>3. Rencana Pelaksanaan Pembelajaran (RPP) disederhanakan
-4. Sistem Zonasi tetap dipakai dengan penyempurnaan
-#pendidikan
-#NadiemMakarim</t>
-  </si>
-  <si>
-    <t>Harusnya dari dulu nih yg kaya gini.https://www.profesiguru.org/2019/12/komponen-inti-format-rpp-terbaru-dari-nadiem.html?m=1 …</t>
-  </si>
-  <si>
-    <t>Dalam kurikulum 2013 Sekolah Dasar
-- Satu Doc pembelajaran RPP = 20 Hal.
-- Satu Sub Tema 6 Pembelajaran
-20 x 6 = 120 Halaman
-- Satu Tema ada 4 Sub Tema
-120 Hal x 4 = 480 Halaman
-- Satu Tahun pembelajaran ada (Max) 9 Tema
-480 Hal x 9 = 4320 Halaman.
-Wkwkwkwk~</t>
-  </si>
-  <si>
-    <t>Apa kurikulum juga akan di sederhanakan? Pengisian raport yang lebih sederhana dan pencairan TF, lebih tepat waktu</t>
-  </si>
-  <si>
-    <t>Bagaimana dengan kurikulum nya pak,,memang ada kelemahan dan kelebihan di setiap kurikulum,,tp menurut saya KTSP lebih banyak pembahasannya dan anak² masih bisa belajar di rumah pelajaran yg di sampaikan dan bisa mempelajari pelajaran yg akan datang,</t>
-  </si>
-  <si>
-    <t>Sederhana kan juga rapor K13 pak menteri</t>
-  </si>
-  <si>
-    <t>Smoga jg pengisian e rapor disederhanakan..</t>
-  </si>
-  <si>
-    <t>Sudah bisa berlaku d semester genap inikah? 😁</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Moga2 gaji nya gak di sederhanakan ya pak mentri </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>😂</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. Kalau jam buat sertifikasi di sederhanakan gpp lah pak mentri </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>😃</t>
-    </r>
-  </si>
-  <si>
-    <t>Kalo sdh sederhana.... opsinya tinggal 2, "bikin" dan "tidak bikin"</t>
-  </si>
-  <si>
-    <t>Rencana pelaksanaan pembelajaran, jadi guru itu kalo mau ngajar harus buat rpp dulu ga lsg msk ngelas ngasih materi. Di rpp ada apa aka yg mau diajarkan, tujuan pembelajaran dll sampe di rppnya ada naskah runtutan waktu ngajar dari doa salam sampe selesai gitu</t>
-  </si>
-  <si>
-    <t>Lbh sdrhan dikit Mbuat tujuan pmbelajaran ya tetep lht KI KD dan buat indikator dulu. Kalo g lihat KI KD, y dokumen kurikulum yg skrag museumkn sj Kalo mau keg blajar jelas n tuntas yg mncerminkn keg siswa y tetep pake sintaks model ato mnimal awal inti akhir Penilaian y jg gitu</t>
-  </si>
-  <si>
-    <t>alhamdulillah kerja guru menjadi ringan</t>
-  </si>
-  <si>
-    <t>setuju disederhanakan, kerja guru ringan</t>
-  </si>
-  <si>
-    <t>secara teori.. secara praktek pembelajarannya rpp yang holistik dan kaffah ternyata jauh dari harapan.. pendidikan sudah mengalami kumunduran karena administrasi yang unfaedah..</t>
-  </si>
-  <si>
-    <t>kegiatan administrasi itu selain fungsi merencanakan secara tertulis juga mengorganisasi, melaksanakan dan mengevaluasi. Mendidik mengajar ...itu sebuah kegiatan yg memerlukan administrasi.</t>
-  </si>
-  <si>
-    <t>Tolong jgn hanya RPP pa mentri, banyak administrasi lain jg yg di rampingkan.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Penilaian Kurikulum 2013 juga tolong ditinjau kembali Pak.
-Kalau bisa dihapus saja..</t>
-  </si>
-  <si>
-    <t>Benar secara Adm tertulis beban guru berkurang. Tapi guru berkompeten tak akan menghilangkan komponen yang dikurangi.Memang kita bisa mengetahui pohon hanya dari buahnya saja namun tak komprehensif.</t>
-  </si>
-  <si>
-    <t>Tolong raport ditinjau, sangat adminstratif sekali....</t>
-  </si>
-  <si>
-    <t>Mudah2an gajinya g ikut disederhanakan dan guru dsuruh hdup sderhana. 😊</t>
-  </si>
-  <si>
-    <t>Harusnya juga lapor tu cukup stu lembar aja krena klw bnyak lembaranya ngehabisin dana juga</t>
-  </si>
-  <si>
-    <t>Harusnya Yg disederhanakn itu penilaiannya.</t>
-  </si>
-  <si>
-    <t>Saya mau kurikulum 2013 dihentikan aja lah...</t>
-  </si>
-  <si>
-    <t>Disederhanakan apa tdk itu tergsntung gurunya..</t>
-  </si>
-  <si>
-    <t>Waduuh 🙄,
-Dlm kegiatan pembelajaran, ada model pembelajaran, beserta sintak2 nya, cukupkah 1 lembar,
-Tambahlah atu lg 🤣🤣🤣🤣</t>
-  </si>
-  <si>
-    <t>Ganti rpp ganti buku cetak lg,ganti trz piye g bingong gurune lan ank murite</t>
-  </si>
-  <si>
-    <t>RPP disederhanakan tpi di penilaiannya tidak disederhnkn y sama saja..</t>
-  </si>
-  <si>
-    <t>Penilaian harusnya juga diaederhakan. Bukan per KD... Kemeng paakk...</t>
-  </si>
-  <si>
-    <t>Bila guru sdh memahami, tanpa selembar formatpun tdk ada persoalan. Format itu hanya cara2 kerja gurita birokrasi mecengkram guru dan siswa.</t>
-  </si>
-  <si>
-    <t>Kita tunggu juknis dan contoh kongkritnya mas Nadiem</t>
-  </si>
-  <si>
-    <t>Yes setuju dengan Assessment jadi kita bisa tau kemampuan dan keahlian anak ada dimana , Great Job</t>
-  </si>
-  <si>
-    <t>Good movement, Pak Nadiem</t>
-  </si>
-  <si>
-    <t>Alhamdulillah, tapi pasti ada pengganti nya</t>
-  </si>
-  <si>
-    <t>Gasssss terosss pak</t>
-  </si>
-  <si>
-    <t>Asal jangan etika &amp; adab diabaikan...</t>
-  </si>
-  <si>
-    <t>I luv u bapak. Bapake peka</t>
-  </si>
-  <si>
-    <t>Mentri millenial gives what millenials want isn it?</t>
-  </si>
-  <si>
-    <t>semoga segenap upaya yang sedang dijalankan dapat berguna bagi bangsa dan negara.</t>
-  </si>
-  <si>
-    <t>Semoga dengan kebijakan ini karakter dan akhlak anak bangsa menjadi lebih baik lagi... sukses Indonesia Maju</t>
-  </si>
-  <si>
-    <t>Semoga pendidikan lebih baik. Kemajuan zaman akan terus bergerak. Akankah kita tidak melesat maju pula?</t>
-  </si>
-  <si>
-    <t>Semoga kebijakan yang ada mampu membawa pendidikan Indonesia lebih baik</t>
-  </si>
-  <si>
-    <t>Semoga kebijakan ini membawa Indonesia lebih maju, #merdeka belajar 💪</t>
-  </si>
-  <si>
-    <t>Kami dukung penuh "change champion" pendidikan Indonesia , #kelasataplangitindonesia</t>
-  </si>
-  <si>
-    <t>Asasmen kompetensi minimum dan survei karakter,mendsetnya(pola pikir) yg bagus utk kemajuan pendidikan kedepan.Harus ada pelatihan utk pengawas/kepala sekolah secara terbimbing dan terstruktur sehingga tujuan pendidikan indonesia bisa tercapai secara maksimal.</t>
-  </si>
-  <si>
-    <t>Langkah tepat, ditunggu langkaglh selanjutnya!</t>
-  </si>
-  <si>
-    <r>
-      <t>Kami dukung, pendidikan jaman old sdh kadaluarsa, tak perlu menghapal krn tinggal google. Olah literasi dr apa yg dibaca dr internet dan literatur, itu mmg yg diperlukan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>👍👍👍</t>
-    </r>
-  </si>
-  <si>
-    <t>Good buat Pak Menteri, Guru itu pendidik bukan administrator.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Merdeka belajar, semoga Siswa tidak terbebani dengan nilai yg sempurna karena pada dasarnya para siswa memiliki kelebihan dn kekurangan masing-masing maka tanggung jawab guru dan orang tua untuk mengolah hasil pembeelajaran siswa.... </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peran guru sebagai pendidik akan lebih "merdeka" menghantarkan anak didiknya menjadi lebih berbudi pekerti luhur, cerdas, kreatif, inovatif dan mandiri. Oknum pendidik yang tidak paham akan esensi pendidikan akan nampak kalang kabut mempersiapkan diri utk mengajar. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surat ke Nadiem, Guru se-Jabar Dukung UN dan USBN Ditiadakan </t>
-  </si>
-  <si>
-    <t>Setuju pak Nadiem ! Sekolah untuk belajar, belajar bukan tempat berkompetisi . Ada saat/waktunya kapan berkompetisi .</t>
-  </si>
-  <si>
-    <t>Ujian online yang sangat mendebarkan dihapus, Alhamdulillah</t>
-  </si>
-  <si>
-    <t>Bagus pak saya setuju,, itu artinya bapak sudah menghapuskan kedzaliman di tanah air kita,, semangat pak lanjutkan,,</t>
-  </si>
-  <si>
-    <t>Saya guru dan saya tidak sabar lagi untuk perubahan ini ...</t>
-  </si>
-  <si>
-    <t>Menteri Dikbud, Nadiem Makarim menetapkan 4 pokok kebijakan pendidikan baru meliputi perbaikan ttg USBN, UN, RPP, dan sistem Zonasi. @Kemdikbud_RI</t>
-  </si>
-  <si>
-    <t>Beberapa hari yang lalu, Menteri Pendidikan dan Kebudayaan telah menetapkan empat program pokok kebijakan pendidikan Merdeka Belajar. Program tersebut meliputi Ujian Sekolah Berstandar Nasional (USBN), Ujian Nasional (UN), pic.twitter.com/j3CAFlfXcp</t>
-  </si>
-  <si>
-    <t>4 pokok Merdeka Belajar,
-1. UN 20121 diubah menjadi Asesmen Kompetensi Minimum dan Survei Karakter
-2. USBN 2020 diterapkan dengan ujian yg diselenggarakan hanya oleh sekolah
-3. Penulisan RPP yg lebih efisien
-4. Sistem zonasi yg lebih fleksibel
-#MerdekaBelajar
-#NadiemMakarim pic.twitter.com/jqWLX8csdn</t>
-  </si>
-  <si>
-    <t>Nadiem Makarim menyampaikan empat program pokok kebijakan pendidikan Merdeka Belajar, yaitu USBN, UN, RPP dan PPDB
-http://bit.ly/2rtENXe</t>
-  </si>
-  <si>
-    <t>Ini Konsep Baru UN dan USBN versi "Merdeka Belajar" Mendikbud Makarim - http://Kompas.com  - Edukasi http://Kompas.com  http://dlvr.it/RL6BxJ  pic.twitter.com/O8X16nk7TQ</t>
-  </si>
-  <si>
-    <t>Lewat arah kebijakan pendidikan "Merdeka Belajar", Mendikbud Nadiem menghapus UN 2021 dan mengubah format USBN 2020. Ini perbedaanya. http://dlvr.it/RL3kJQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ada 4 program pokok dalam Kebijakan Pendidikan "Merdeka Belajar" yang ditetapkan Nadiem Makarim hari ini. Apa saja? </t>
-  </si>
-  <si>
-    <t>Siaran Pers Kemdikbud Nomor: 408/sipres/A5.3/XII/2019 tentang "merdeka belajar" itu didefinisikan sebagai berikut:
-1. USBN 2020 dilaksanakan oleh sekolah untuk menilai kompetensi siswa dalam bentuk tes tulis...</t>
-  </si>
-  <si>
-    <t>"Program tersebut meliputi Ujian Sekolah Berstandar Nasional (USBN), Ujian Nasional ( UN), Rencana Pelaksanaan Pembelajaran (RPP), dan Peraturan Penerimaan Peserta Didik Baru (PPDB) Zonasi,"
- #HukumPerusuhNegeri</t>
-  </si>
-  <si>
-    <t>Mendikbud Nadiem Makarim sudah menetapkan program pokok kebijakan pendidikan, terkait USBN, Ujian Nasional alias UN, RPP, dan PPDB Zonasi, disebut Merdeka Belajar. #ProgramNadiemMakarim http://m.jpnn.com/news/4-program-pokok-mendikbud-nadiem-makarim-merdeka-belajar …</t>
-  </si>
-  <si>
-    <t>Empat fokus kebijakan Merdeka belajar terkait Ujian Sekolah Berstandar Nasional (USBN), Ujian Nasional ( UN), Rencana Pelaksanaan Pembelajaran (RPP), dan Peraturan Penerimaan Peserta Didik Baru (PPDB) Zonasi. #POLEMIKHapusUN</t>
-  </si>
-  <si>
-    <t>@WikiDPR #Kom10 Nadiem, Mendikbud: pokok pokok kebijakan merdeka belajar yaitu:
-1. Ujian Sekolah Berstandar Nasional (USBN).
-2. Ujian Nasional.
-3. Recana Pelaksanaan Pembelajaran (RPP).
-4. Peraturan Penerimaan Peserta Didik Baru (PPDP) Zonasi.</t>
-  </si>
-  <si>
-    <t>Menteri Pendidikan dan Kebudayaan, Nadiem Makarim menetapkan empat program kebijakan pendidikan dengan nama "Merdeka Belajar" yang meliputi Ujian Sekolah Berstandar Nasional (USBN) dan Ujian Nasional (UN)
-.
-Kebijakan… https://www.instagram.com/p/B59c2YonLj7/?igshid=u1t4bdvnafoa …</t>
-  </si>
-  <si>
-    <t>Inti kebijakan merdeka belajar yang ditetapkan Nadiem Makarim adalah:
-1. Ujian Sekolah Berstandar Nasional (USBN) akan digunakan untuk mengukur kompetensi siswa
-2. Ujian Nasional (UN) dihentikan, diganti Asesmen Kompetensi Minimum dan Survei Karakter di kelas 4, 8, dan 11
-(3/4)</t>
-  </si>
-  <si>
-    <t>Nadiem Makarim: Empat program pokok kebijakan pendidikan, meliputi perubahan pada USBN, UN, RPP, dan PPDB Zonasi.
-#Peristiwa #Belajar #Merdeka #NadiemMakaraim #Mendikbud
-https://www.netralnews.com/peristiwa/read/196232/begini-cara-belajar-merdeka-ala-nadiem …</t>
-  </si>
-  <si>
-    <t>"Program tersebut meliputi Ujian Sekolah Berstandar Nasional (USBN), Ujian Nasional ( UN), Rencana Pelaksanaan Pembelajaran (RPP), dan Peraturan Penerimaan Peserta Didik Baru (PPDB) Zonasi," ujar Nadiem.
-https://nasional.kompas.com/read/2019/12/11/11244621/nadiem-makarim-tetapkan-program-merdeka-belajar-salah-satunya-hapus-un …</t>
-  </si>
-  <si>
-    <t>Empat program pokok kebijakan pendidikan 'Merdeka Belajar' itu:
-1. Ujian Sekolah Berstandar Nasional (USBN)
-2. Ujian Nasional (UN)
-3. Rencana Pelaksanaan Pembelajaran (RPP)
-4. Peraturan Penerimaan Peserta Didik Baru (PPDB) Zonasi.</t>
-  </si>
-  <si>
-    <t>Bukannya sama aja ya...UN maupun USBN?</t>
-  </si>
-  <si>
-    <t>Klean pernah sekolah bukan? Pernah ujian bukan? Ya gitu deh, kura kura dalam perahu</t>
-  </si>
-  <si>
-    <t>Ujian hanya instrument alat ukur hasil belajar, bukan elemen pembangun kualitas intelegensi bung @Kemdikbud_RI.
-Mana Materi Kurikulum Program Pembinaan Moral?
-Haadeehh..
-Mas @jokowi Eyang @trahkartasura Bro @relawanperak2 Jeng @msoekarnoputri gimana nih?
-https://edukasi.kompas.com/read/2019/12/11/14433351/ini-konsep-baru-un-dan-usbn-versi-merdeka-belajar-mendikbud-makarim …</t>
-  </si>
-  <si>
-    <t>Skripsi di hapus dan di ganti dengan studi keluar negri.</t>
-  </si>
-  <si>
-    <t>Nglamar kerja ga pake ijazah. Daftar kuliah ga pake ijazah.</t>
-  </si>
-  <si>
-    <t>yaallah, knp ga 2020 aj :(</t>
-  </si>
-  <si>
-    <t>Ngopo ra ket mbien</t>
-  </si>
-  <si>
-    <t>Nek taon iki wae pizee?</t>
-  </si>
-  <si>
-    <t>kenapa gak 2020 aja kalo 2021 gua dah lulus</t>
-  </si>
-  <si>
-    <t>Smoga bukan sekedar wacana saja</t>
-  </si>
-  <si>
-    <t>Yah namanya GK seru klo gtu... Enak banget dong GK ada Terget?</t>
-  </si>
-  <si>
-    <t>Kenapa sih angkatan saya selalu menjadi bahan percobaan anjay lah</t>
-  </si>
-  <si>
-    <t>Kebijakan dlm dunia pendidikan kita persis spt perilaku kumbang. Singgah sesaat lalu beralih ke yg baru.</t>
-  </si>
-  <si>
-    <t>Mbok yg dihapus itu bayar SPP. Mentri baru kok ga ada yg baru</t>
-  </si>
-  <si>
-    <t>Tolong gobloknya jangan diambil semua gini dong mas</t>
-  </si>
-  <si>
-    <t>Kalo begini ini guru juga harus mempunnyai kemampuan lebih utk mengakomodir seluruh persoalan Murid'Muridnya</t>
-  </si>
-  <si>
-    <t>Semoga ada perubahan kurikulum.yg lebih sesuai dengan kemampuan, karakter dan kondisi bangsa indonesia. Bukan asal comot kurikulum dari luar negeri entah itu dari finlandia ato dari manapun juga.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Kurtilas ya kurikulum tiga belas... Haduh isinya udah kaya gado2x Campur2x </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>🙈</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>...</t>
-    </r>
-  </si>
-  <si>
-    <t>Sekolah seminggu 6hari aktif harusnya dikurangi menjadi 4 hari karena kasihan siswa terbebani mikir pelajaran atau kalo perlu masuknya seminggu sekali saja😁</t>
-  </si>
-  <si>
-    <t>Jika UN Dihapuskan maka tidak ada tolak ukur untuk mengukur kemampuan dan kemajuan akademis siswa.!!!!!!!!! Dan jika hnya sebatas ujian sekolah. Pastinya tidak akan fear ( (tidak murni nilai hasil kemampuan siswa) yg pasti tidak akan berstandar nasional) bagaimmana mau pemetaan kompetensi klo UN ato USBN tidak ada....</t>
-  </si>
-  <si>
-    <t>kalau un di hapus , mau ndaftar universitas dan kerja patokannya apa y pak ? maaf saya belum jelas</t>
-  </si>
-  <si>
-    <t>Harusnya 50 thn yg lalu sdh harus begini...</t>
-  </si>
-  <si>
-    <t>Terus gimana ya cara penilaian survei karakter...apakah penilaiannya bisa objektif? UN yang sekarang kan tidak menentukan kelulusan...sebenarnya sudah tidak membebani...ya semoga saja UN di ganti dengan Asasmen kompetensi...tidak menurunkan semangat belajar siswa...karena tidak ada UN jadi tidak belajar...</t>
-  </si>
-  <si>
-    <t>Guru yang waktu ngajar main hp pecat saja ...guru sekarang banyak yang malas ...</t>
-  </si>
-  <si>
-    <t>Gonta ganti kebijakan melulu, guru bingung, murid ga tau tujuan pembelajaran buat apa. Pengangguran pribumi banyak.</t>
-  </si>
-  <si>
-    <t>Katany un itu adalah amanat undang-undang pak. Kudu revisi undang-undang dulu.</t>
-  </si>
-  <si>
-    <t>Semoga tdk hanya berganti istilahnya saja, USBN &amp; UN tak jauh berbeda....</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Yah...yg ujian nya di 2020 hrs teteup UN doong </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>😭</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Kasiihan anakku stress</t>
-    </r>
-  </si>
-  <si>
-    <t>Gak ada lagi dana UN donk, gmn nasib dpr.??</t>
-  </si>
-  <si>
-    <t>Ganti mentri ganti program,. ganti buku,.. gant modul,. ganti dan ganti.... apa enggak sebaiknya memperbaiki yg sudah ada atau menambah yg belum agar lengkap... semua kan butuh biaya...</t>
-  </si>
-  <si>
-    <r>
-      <t>Yaaah 2020 doong pak Menteri</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>😭😭</t>
-    </r>
-  </si>
-  <si>
-    <t>Sudah bagus namanya Ujian Nasional kok malah diganti assessment kompetensi.. Ingat sumpah pemuda kalo kita memang cinta Indonesia. " Berbahasa yang satu bahasa Indonesia.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yg di perhatikan ujiannya
-Proses menuju ujian itu sdh diperhatikan blm? Kok Tau2 ngubah ujiannya... </t>
-  </si>
-  <si>
-    <t>Pak...bukankah USBN sudah bukan satu2nya faktor penentu kelulusan???! Selama ini kelulusan juga SUDAH ditentukan oleh guru dan sekolah masing-masing pak. Jadi USBN membatasinya di sisi mana???</t>
-  </si>
-  <si>
-    <t>Isi pelajarannya dikurangi pak</t>
-  </si>
-  <si>
-    <t>Dukung pak mendikbud, UN bkn satu2nya tolak ukur kelulusan siswa</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9962,20 +8832,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFDB831C"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -10382,8 +9238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1296" workbookViewId="0">
-      <selection activeCell="D1301" sqref="D1301"/>
+    <sheetView tabSelected="1" topLeftCell="D990" workbookViewId="0">
+      <selection activeCell="F1002" sqref="F1002"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30414,2745 +29270,1245 @@
     </row>
     <row r="1002" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1002" s="6"/>
-      <c r="D1002" s="5" t="s">
-        <v>2743</v>
-      </c>
-      <c r="F1002" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1003" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1002" s="5"/>
+    </row>
+    <row r="1003" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1003" s="6"/>
-      <c r="D1003" s="5" t="s">
-        <v>2744</v>
-      </c>
-      <c r="F1003" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1004" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="D1003" s="5"/>
+    </row>
+    <row r="1004" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1004" s="6"/>
-      <c r="D1004" s="5" t="s">
-        <v>2745</v>
-      </c>
-      <c r="F1004" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1004" s="5"/>
     </row>
     <row r="1005" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1005" s="6"/>
-      <c r="D1005" s="5" t="s">
-        <v>2746</v>
-      </c>
-      <c r="F1005" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1005" s="5"/>
     </row>
     <row r="1006" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1006" s="6"/>
-      <c r="D1006" s="5" t="s">
-        <v>2747</v>
-      </c>
-      <c r="F1006" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1006" s="5"/>
     </row>
     <row r="1007" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1007" s="6"/>
-      <c r="D1007" s="5" t="s">
-        <v>2748</v>
-      </c>
-      <c r="F1007" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1007" s="5"/>
     </row>
     <row r="1008" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1008" s="6"/>
-      <c r="D1008" s="5" t="s">
-        <v>3033</v>
-      </c>
-      <c r="F1008" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1009" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1008" s="5"/>
+    </row>
+    <row r="1009" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1009" s="6"/>
-      <c r="D1009" s="5" t="s">
-        <v>2749</v>
-      </c>
-      <c r="F1009" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1010" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1009" s="5"/>
+    </row>
+    <row r="1010" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1010" s="6"/>
-      <c r="D1010" s="5" t="s">
-        <v>3034</v>
-      </c>
-      <c r="F1010" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1011" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1010" s="5"/>
+    </row>
+    <row r="1011" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1011" s="6"/>
-      <c r="D1011" s="5" t="s">
-        <v>2750</v>
-      </c>
-      <c r="F1011" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1012" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1011" s="5"/>
+    </row>
+    <row r="1012" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1012" s="6"/>
-      <c r="D1012" s="5" t="s">
-        <v>2751</v>
-      </c>
-      <c r="F1012" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1013" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="D1012" s="5"/>
+    </row>
+    <row r="1013" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1013" s="6"/>
-      <c r="D1013" s="5" t="s">
-        <v>2752</v>
-      </c>
-      <c r="F1013" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1014" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1013" s="5"/>
+    </row>
+    <row r="1014" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1014" s="6"/>
-      <c r="D1014" s="5" t="s">
-        <v>2753</v>
-      </c>
-      <c r="F1014" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1015" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1014" s="5"/>
+    </row>
+    <row r="1015" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1015" s="6"/>
-      <c r="D1015" s="5" t="s">
-        <v>2754</v>
-      </c>
-      <c r="F1015" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1016" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1015" s="5"/>
+    </row>
+    <row r="1016" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1016" s="6"/>
-      <c r="D1016" s="5" t="s">
-        <v>2755</v>
-      </c>
-      <c r="F1016" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1017" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1016" s="5"/>
+    </row>
+    <row r="1017" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1017" s="6"/>
-      <c r="D1017" s="5" t="s">
-        <v>2756</v>
-      </c>
-      <c r="F1017" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1018" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1017" s="5"/>
+    </row>
+    <row r="1018" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1018" s="6"/>
-      <c r="D1018" s="5" t="s">
-        <v>2757</v>
-      </c>
-      <c r="F1018" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1019" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1018" s="5"/>
+    </row>
+    <row r="1019" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1019" s="6"/>
-      <c r="D1019" s="5" t="s">
-        <v>2758</v>
-      </c>
-      <c r="F1019" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1020" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1019" s="5"/>
+    </row>
+    <row r="1020" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1020" s="6"/>
-      <c r="D1020" s="5" t="s">
-        <v>2759</v>
-      </c>
-      <c r="F1020" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1021" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1020" s="5"/>
+    </row>
+    <row r="1021" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1021" s="6"/>
-      <c r="D1021" s="5" t="s">
-        <v>2760</v>
-      </c>
-      <c r="F1021" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1022" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1021" s="5"/>
+    </row>
+    <row r="1022" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1022" s="6"/>
-      <c r="D1022" s="5" t="s">
-        <v>2761</v>
-      </c>
-      <c r="F1022" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1023" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1022" s="5"/>
+    </row>
+    <row r="1023" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1023" s="6"/>
-      <c r="D1023" s="5" t="s">
-        <v>2762</v>
-      </c>
-      <c r="F1023" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1024" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1023" s="5"/>
+    </row>
+    <row r="1024" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1024" s="6"/>
-      <c r="D1024" s="5" t="s">
-        <v>2763</v>
-      </c>
-      <c r="F1024" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1025" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1024" s="5"/>
+    </row>
+    <row r="1025" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1025" s="6"/>
-      <c r="D1025" s="5" t="s">
-        <v>2764</v>
-      </c>
-      <c r="F1025" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1026" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1025" s="5"/>
+    </row>
+    <row r="1026" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1026" s="6"/>
-      <c r="D1026" s="5" t="s">
-        <v>2765</v>
-      </c>
-      <c r="F1026" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1027" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="D1026" s="5"/>
+    </row>
+    <row r="1027" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1027" s="6"/>
-      <c r="D1027" s="5" t="s">
-        <v>2766</v>
-      </c>
-      <c r="F1027" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1028" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1027" s="5"/>
+    </row>
+    <row r="1028" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1028" s="6"/>
-      <c r="D1028" s="5" t="s">
-        <v>2767</v>
-      </c>
-      <c r="F1028" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1029" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1028" s="5"/>
+    </row>
+    <row r="1029" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1029" s="6"/>
-      <c r="D1029" s="5" t="s">
-        <v>2768</v>
-      </c>
-      <c r="F1029" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1030" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1029" s="5"/>
+    </row>
+    <row r="1030" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1030" s="6"/>
-      <c r="D1030" s="5" t="s">
-        <v>2769</v>
-      </c>
-      <c r="F1030" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1031" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1030" s="5"/>
+    </row>
+    <row r="1031" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1031" s="6"/>
-      <c r="D1031" s="5" t="s">
-        <v>2770</v>
-      </c>
-      <c r="F1031" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1032" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1031" s="5"/>
+    </row>
+    <row r="1032" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1032" s="6"/>
-      <c r="D1032" s="5" t="s">
-        <v>2771</v>
-      </c>
-      <c r="F1032" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1033" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1032" s="5"/>
+    </row>
+    <row r="1033" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1033" s="6"/>
-      <c r="D1033" s="5" t="s">
-        <v>2772</v>
-      </c>
-      <c r="F1033" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1034" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1033" s="5"/>
+    </row>
+    <row r="1034" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1034" s="6"/>
-      <c r="D1034" s="5" t="s">
-        <v>2773</v>
-      </c>
-      <c r="F1034" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1035" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1034" s="5"/>
+    </row>
+    <row r="1035" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1035" s="6"/>
-      <c r="D1035" s="5" t="s">
-        <v>2774</v>
-      </c>
-      <c r="F1035" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1036" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1035" s="5"/>
+    </row>
+    <row r="1036" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1036" s="6"/>
-      <c r="D1036" s="5" t="s">
-        <v>2775</v>
-      </c>
-      <c r="F1036" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1037" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1036" s="5"/>
+    </row>
+    <row r="1037" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1037" s="6"/>
-      <c r="D1037" s="5" t="s">
-        <v>2776</v>
-      </c>
-      <c r="F1037" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1038" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1037" s="5"/>
+    </row>
+    <row r="1038" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1038" s="6"/>
-      <c r="D1038" s="5" t="s">
-        <v>2777</v>
-      </c>
-      <c r="F1038" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1039" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1038" s="5"/>
+    </row>
+    <row r="1039" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1039" s="6"/>
-      <c r="D1039" s="5" t="s">
-        <v>2778</v>
-      </c>
-      <c r="F1039" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1040" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1039" s="5"/>
+    </row>
+    <row r="1040" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1040" s="6"/>
-      <c r="D1040" s="5" t="s">
-        <v>2779</v>
-      </c>
-      <c r="F1040" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1041" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1040" s="5"/>
+    </row>
+    <row r="1041" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1041" s="6"/>
-      <c r="D1041" s="5" t="s">
-        <v>2780</v>
-      </c>
-      <c r="F1041" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1042" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1041" s="5"/>
+    </row>
+    <row r="1042" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1042" s="6"/>
-      <c r="D1042" s="5" t="s">
-        <v>2781</v>
-      </c>
-      <c r="F1042" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1043" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1042" s="5"/>
+    </row>
+    <row r="1043" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1043" s="6"/>
-      <c r="D1043" s="5" t="s">
-        <v>2782</v>
-      </c>
-      <c r="F1043" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1044" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1043" s="5"/>
+    </row>
+    <row r="1044" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1044" s="6"/>
-      <c r="D1044" s="5" t="s">
-        <v>2783</v>
-      </c>
-      <c r="F1044" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1045" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1044" s="5"/>
+    </row>
+    <row r="1045" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1045" s="6"/>
-      <c r="D1045" s="5" t="s">
-        <v>2784</v>
-      </c>
-      <c r="F1045" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1046" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1045" s="5"/>
+    </row>
+    <row r="1046" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1046" s="6"/>
-      <c r="D1046" s="5" t="s">
-        <v>2785</v>
-      </c>
-      <c r="F1046" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1047" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1046" s="5"/>
+    </row>
+    <row r="1047" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1047" s="6"/>
-      <c r="D1047" s="5" t="s">
-        <v>2786</v>
-      </c>
-      <c r="F1047" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1048" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1047" s="5"/>
+    </row>
+    <row r="1048" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1048" s="6"/>
-      <c r="D1048" s="5" t="s">
-        <v>2787</v>
-      </c>
-      <c r="F1048" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1049" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1048" s="5"/>
+    </row>
+    <row r="1049" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1049" s="6"/>
-      <c r="D1049" s="5" t="s">
-        <v>2788</v>
-      </c>
-      <c r="F1049" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1050" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="D1049" s="5"/>
+    </row>
+    <row r="1050" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1050" s="6"/>
-      <c r="D1050" s="5" t="s">
-        <v>2789</v>
-      </c>
-      <c r="F1050" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1051" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1050" s="5"/>
+    </row>
+    <row r="1051" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1051" s="6"/>
-      <c r="D1051" s="5" t="s">
-        <v>2790</v>
-      </c>
-      <c r="F1051" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1052" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1051" s="5"/>
+    </row>
+    <row r="1052" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1052" s="6"/>
-      <c r="D1052" s="5" t="s">
-        <v>2791</v>
-      </c>
-      <c r="F1052" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1053" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1052" s="5"/>
+    </row>
+    <row r="1053" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1053" s="6"/>
-      <c r="D1053" s="5" t="s">
-        <v>2792</v>
-      </c>
-      <c r="F1053" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1054" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1053" s="5"/>
+    </row>
+    <row r="1054" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1054" s="6"/>
-      <c r="D1054" s="5" t="s">
-        <v>2793</v>
-      </c>
-      <c r="F1054" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1055" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1054" s="5"/>
+    </row>
+    <row r="1055" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1055" s="6"/>
-      <c r="D1055" s="5" t="s">
-        <v>2794</v>
-      </c>
-      <c r="F1055" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1056" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1055" s="5"/>
+    </row>
+    <row r="1056" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1056" s="6"/>
-      <c r="D1056" s="5" t="s">
-        <v>2795</v>
-      </c>
-      <c r="F1056" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1057" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1056" s="5"/>
+    </row>
+    <row r="1057" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1057" s="6"/>
-      <c r="D1057" s="5" t="s">
-        <v>2796</v>
-      </c>
-      <c r="F1057" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1058" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1057" s="5"/>
+    </row>
+    <row r="1058" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1058" s="6"/>
-      <c r="D1058" s="5" t="s">
-        <v>2797</v>
-      </c>
-      <c r="F1058" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1059" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1058" s="5"/>
+    </row>
+    <row r="1059" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1059" s="6"/>
-      <c r="D1059" s="5" t="s">
-        <v>2798</v>
-      </c>
-      <c r="F1059" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1060" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1059" s="5"/>
+    </row>
+    <row r="1060" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1060" s="6"/>
-      <c r="D1060" s="5" t="s">
-        <v>2799</v>
-      </c>
-      <c r="F1060" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1061" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1060" s="5"/>
+    </row>
+    <row r="1061" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1061" s="6"/>
-      <c r="D1061" s="5" t="s">
-        <v>2800</v>
-      </c>
-      <c r="F1061" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1062" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1061" s="5"/>
+    </row>
+    <row r="1062" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1062" s="6"/>
-      <c r="D1062" s="5" t="s">
-        <v>2801</v>
-      </c>
-      <c r="F1062" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1063" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1062" s="5"/>
+    </row>
+    <row r="1063" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1063" s="6"/>
-      <c r="D1063" s="5" t="s">
-        <v>2802</v>
-      </c>
-      <c r="F1063" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1064" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1063" s="5"/>
+    </row>
+    <row r="1064" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1064" s="6"/>
-      <c r="D1064" s="5" t="s">
-        <v>2803</v>
-      </c>
-      <c r="F1064" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1065" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1064" s="5"/>
+    </row>
+    <row r="1065" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1065" s="6"/>
-      <c r="D1065" s="5" t="s">
-        <v>2804</v>
-      </c>
-      <c r="F1065" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1066" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1065" s="5"/>
+    </row>
+    <row r="1066" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1066" s="6"/>
-      <c r="D1066" s="5" t="s">
-        <v>2805</v>
-      </c>
-      <c r="F1066" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1067" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1066" s="5"/>
+    </row>
+    <row r="1067" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1067" s="6"/>
-      <c r="D1067" s="5" t="s">
-        <v>2806</v>
-      </c>
-      <c r="F1067" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1068" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="D1067" s="5"/>
+    </row>
+    <row r="1068" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1068" s="6"/>
-      <c r="D1068" s="5" t="s">
-        <v>2807</v>
-      </c>
-      <c r="F1068" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1069" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1068" s="5"/>
+    </row>
+    <row r="1069" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1069" s="6"/>
-      <c r="D1069" s="5" t="s">
-        <v>2808</v>
-      </c>
-      <c r="F1069" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1070" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1069" s="5"/>
+    </row>
+    <row r="1070" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1070" s="6"/>
-      <c r="D1070" s="5" t="s">
-        <v>2809</v>
-      </c>
-      <c r="F1070" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1071" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1070" s="5"/>
+    </row>
+    <row r="1071" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1071" s="6"/>
-      <c r="D1071" s="5" t="s">
-        <v>2810</v>
-      </c>
-      <c r="F1071" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1072" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1071" s="5"/>
+    </row>
+    <row r="1072" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1072" s="6"/>
-      <c r="D1072" s="5" t="s">
-        <v>2811</v>
-      </c>
-      <c r="F1072" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1073" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1072" s="5"/>
+    </row>
+    <row r="1073" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1073" s="6"/>
-      <c r="D1073" s="5" t="s">
-        <v>2812</v>
-      </c>
-      <c r="F1073" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1074" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1073" s="5"/>
+    </row>
+    <row r="1074" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1074" s="6"/>
-      <c r="D1074" s="5" t="s">
-        <v>2813</v>
-      </c>
-      <c r="F1074" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1075" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1074" s="5"/>
+    </row>
+    <row r="1075" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1075" s="6"/>
-      <c r="D1075" s="5" t="s">
-        <v>2814</v>
-      </c>
-      <c r="F1075" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1076" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1075" s="5"/>
+    </row>
+    <row r="1076" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1076" s="6"/>
-      <c r="D1076" s="5" t="s">
-        <v>2815</v>
-      </c>
-      <c r="F1076" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1077" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1076" s="5"/>
+    </row>
+    <row r="1077" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1077" s="6"/>
-      <c r="D1077" s="4" t="s">
-        <v>2816</v>
-      </c>
-      <c r="F1077" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1078" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1077" s="4"/>
+    </row>
+    <row r="1078" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1078" s="6"/>
-      <c r="D1078" s="5" t="s">
-        <v>2817</v>
-      </c>
-      <c r="F1078" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1079" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1078" s="5"/>
+    </row>
+    <row r="1079" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1079" s="6"/>
-      <c r="D1079" s="5" t="s">
-        <v>2818</v>
-      </c>
-      <c r="F1079" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1080" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1079" s="5"/>
+    </row>
+    <row r="1080" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1080" s="6"/>
-      <c r="D1080" s="5" t="s">
-        <v>2819</v>
-      </c>
-      <c r="F1080" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1081" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1080" s="5"/>
+    </row>
+    <row r="1081" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1081" s="6"/>
-      <c r="D1081" s="5" t="s">
-        <v>2820</v>
-      </c>
-      <c r="F1081" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1082" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1081" s="5"/>
+    </row>
+    <row r="1082" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1082" s="6"/>
-      <c r="D1082" s="5" t="s">
-        <v>2821</v>
-      </c>
-      <c r="F1082" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1083" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1082" s="5"/>
+    </row>
+    <row r="1083" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1083" s="6"/>
-      <c r="D1083" s="5" t="s">
-        <v>2822</v>
-      </c>
-      <c r="F1083" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1084" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1083" s="5"/>
+    </row>
+    <row r="1084" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1084" s="6"/>
-      <c r="D1084" t="s">
-        <v>2823</v>
-      </c>
-      <c r="F1084" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1085" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1085" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1085" s="6"/>
-      <c r="D1085" t="s">
-        <v>2824</v>
-      </c>
-      <c r="F1085" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1086" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1086" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1086" s="6"/>
-      <c r="D1086" t="s">
-        <v>2825</v>
-      </c>
-      <c r="F1086" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1087" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1087" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1087" s="6"/>
-      <c r="D1087" t="s">
-        <v>2826</v>
-      </c>
-      <c r="F1087" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1088" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1088" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1088" s="6"/>
-      <c r="D1088" t="s">
-        <v>2827</v>
-      </c>
-      <c r="F1088" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1089" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1089" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1089" s="6"/>
-      <c r="D1089" t="s">
-        <v>2828</v>
-      </c>
-      <c r="F1089" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1090" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1090" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1090" s="6"/>
-      <c r="D1090" t="s">
-        <v>2829</v>
-      </c>
-      <c r="F1090" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1091" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1091" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1091" s="6"/>
-      <c r="D1091" s="5" t="s">
-        <v>2830</v>
-      </c>
-      <c r="F1091" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1092" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1091" s="5"/>
+    </row>
+    <row r="1092" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1092" s="6"/>
-      <c r="D1092" s="5" t="s">
-        <v>2831</v>
-      </c>
-      <c r="F1092" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1093" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1092" s="5"/>
+    </row>
+    <row r="1093" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1093" s="6"/>
-      <c r="D1093" s="5" t="s">
-        <v>2832</v>
-      </c>
-      <c r="F1093" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1094" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1093" s="5"/>
+    </row>
+    <row r="1094" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1094" s="6"/>
-      <c r="D1094" s="5" t="s">
-        <v>2833</v>
-      </c>
-      <c r="F1094" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1095" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1094" s="5"/>
+    </row>
+    <row r="1095" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1095" s="6"/>
-      <c r="D1095" s="5" t="s">
-        <v>2834</v>
-      </c>
-      <c r="F1095" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1096" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1095" s="5"/>
+    </row>
+    <row r="1096" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1096" s="6"/>
-      <c r="D1096" s="5" t="s">
-        <v>2835</v>
-      </c>
-      <c r="F1096" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1097" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1096" s="5"/>
+    </row>
+    <row r="1097" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1097" s="6"/>
-      <c r="D1097" s="5" t="s">
-        <v>2836</v>
-      </c>
-      <c r="F1097" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1098" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1097" s="5"/>
+    </row>
+    <row r="1098" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1098" s="6"/>
-      <c r="D1098" s="5" t="s">
-        <v>2837</v>
-      </c>
-      <c r="F1098" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1099" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1098" s="5"/>
+    </row>
+    <row r="1099" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1099" s="6"/>
-      <c r="D1099" s="5" t="s">
-        <v>2838</v>
-      </c>
-      <c r="F1099" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1099" s="5"/>
+    </row>
+    <row r="1100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1100" s="6"/>
-      <c r="D1100" s="5" t="s">
-        <v>2839</v>
-      </c>
-      <c r="F1100" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1100" s="5"/>
+    </row>
+    <row r="1101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1101" s="6"/>
-      <c r="D1101" s="5" t="s">
-        <v>2840</v>
-      </c>
-      <c r="F1101" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1101" s="5"/>
+    </row>
+    <row r="1102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1102" s="6"/>
-      <c r="D1102" s="5" t="s">
-        <v>2841</v>
-      </c>
-      <c r="F1102" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1102" s="5"/>
+    </row>
+    <row r="1103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1103" s="6"/>
-      <c r="D1103" s="5" t="s">
-        <v>2842</v>
-      </c>
-      <c r="F1103" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1103" s="5"/>
+    </row>
+    <row r="1104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1104" s="6"/>
-      <c r="D1104" s="5" t="s">
-        <v>2843</v>
-      </c>
-      <c r="F1104" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1104" s="5"/>
     </row>
     <row r="1105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1105" s="6"/>
-      <c r="D1105" s="5" t="s">
-        <v>2844</v>
-      </c>
-      <c r="F1105" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1105" s="5"/>
+    </row>
+    <row r="1106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1106" s="6"/>
-      <c r="D1106" s="5" t="s">
-        <v>2845</v>
-      </c>
-      <c r="F1106" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1106" s="5"/>
+    </row>
+    <row r="1107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1107" s="6"/>
-      <c r="D1107" s="5" t="s">
-        <v>2846</v>
-      </c>
-      <c r="F1107" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1107" s="5"/>
+    </row>
+    <row r="1108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1108" s="6"/>
-      <c r="D1108" s="5" t="s">
-        <v>2847</v>
-      </c>
-      <c r="F1108" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1108" s="5"/>
+    </row>
+    <row r="1109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1109" s="6"/>
-      <c r="D1109" s="5" t="s">
-        <v>2848</v>
-      </c>
-      <c r="F1109" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1109" s="5"/>
     </row>
     <row r="1110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1110" s="6"/>
-      <c r="D1110" s="5" t="s">
-        <v>2849</v>
-      </c>
-      <c r="F1110" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1111" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1110" s="5"/>
+    </row>
+    <row r="1111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1111" s="6"/>
-      <c r="D1111" s="5" t="s">
-        <v>2850</v>
-      </c>
-      <c r="F1111" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1111" s="5"/>
     </row>
     <row r="1112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1112" s="6"/>
-      <c r="D1112" s="5" t="s">
-        <v>2851</v>
-      </c>
-      <c r="F1112" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1112" s="5"/>
+    </row>
+    <row r="1113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1113" s="6"/>
-      <c r="D1113" s="5" t="s">
-        <v>2852</v>
-      </c>
-      <c r="F1113" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1114" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1113" s="5"/>
+    </row>
+    <row r="1114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1114" s="6"/>
-      <c r="D1114" s="5" t="s">
-        <v>2853</v>
-      </c>
-      <c r="F1114" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1115" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1114" s="5"/>
+    </row>
+    <row r="1115" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1115" s="7"/>
-      <c r="D1115" s="5" t="s">
-        <v>2854</v>
-      </c>
-      <c r="F1115" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1116" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1115" s="5"/>
+      <c r="F1115"/>
+    </row>
+    <row r="1116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1116" s="6"/>
-      <c r="D1116" s="5" t="s">
-        <v>2855</v>
-      </c>
-      <c r="F1116" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1116" s="5"/>
+    </row>
+    <row r="1117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1117" s="6"/>
-      <c r="D1117" s="5" t="s">
-        <v>2856</v>
-      </c>
-      <c r="F1117" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1117" s="5"/>
     </row>
     <row r="1118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1118" s="6"/>
-      <c r="D1118" s="5" t="s">
-        <v>2857</v>
-      </c>
-      <c r="F1118" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1119" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1118" s="5"/>
+    </row>
+    <row r="1119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1119" s="6"/>
-      <c r="D1119" s="5" t="s">
-        <v>2858</v>
-      </c>
-      <c r="F1119" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1120" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1119" s="5"/>
+    </row>
+    <row r="1120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1120" s="6"/>
-      <c r="D1120" s="5" t="s">
-        <v>2859</v>
-      </c>
-      <c r="F1120" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1120" s="5"/>
+    </row>
+    <row r="1121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1121" s="6"/>
-      <c r="D1121" s="5" t="s">
-        <v>2860</v>
-      </c>
-      <c r="F1121" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1121" s="5"/>
+    </row>
+    <row r="1122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1122" s="6"/>
-      <c r="D1122" s="5" t="s">
-        <v>2861</v>
-      </c>
-      <c r="F1122" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1122" s="5"/>
+    </row>
+    <row r="1123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1123" s="6"/>
-      <c r="D1123" s="5" t="s">
-        <v>2862</v>
-      </c>
-      <c r="F1123" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1124" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1123" s="5"/>
+    </row>
+    <row r="1124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1124" s="6"/>
-      <c r="D1124" s="5" t="s">
-        <v>2863</v>
-      </c>
-      <c r="F1124" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1124" s="5"/>
+    </row>
+    <row r="1125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1125" s="6"/>
-      <c r="D1125" s="5" t="s">
-        <v>2864</v>
-      </c>
-      <c r="F1125" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1126" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1125" s="5"/>
+    </row>
+    <row r="1126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1126" s="6"/>
-      <c r="D1126" s="5" t="s">
-        <v>2865</v>
-      </c>
-      <c r="F1126" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1126" s="5"/>
+    </row>
+    <row r="1127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1127" s="6"/>
-      <c r="D1127" s="5" t="s">
-        <v>2866</v>
-      </c>
-      <c r="F1127" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1127" s="5"/>
+    </row>
+    <row r="1128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1128" s="6"/>
-      <c r="D1128" s="5" t="s">
-        <v>2867</v>
-      </c>
-      <c r="F1128" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1128" s="5"/>
+    </row>
+    <row r="1129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1129" s="6"/>
-      <c r="D1129" s="5" t="s">
-        <v>2868</v>
-      </c>
-      <c r="F1129" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1130" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1129" s="5"/>
+    </row>
+    <row r="1130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1130" s="6"/>
-      <c r="D1130" s="5" t="s">
-        <v>2869</v>
-      </c>
-      <c r="F1130" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1130" s="5"/>
+    </row>
+    <row r="1131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1131" s="6"/>
-      <c r="D1131" s="5" t="s">
-        <v>2870</v>
-      </c>
-      <c r="F1131" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1131" s="5"/>
+    </row>
+    <row r="1132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1132" s="6"/>
-      <c r="D1132" s="5" t="s">
-        <v>2871</v>
-      </c>
-      <c r="F1132" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1133" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1132" s="5"/>
+    </row>
+    <row r="1133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1133" s="6"/>
-      <c r="D1133" s="5" t="s">
-        <v>2872</v>
-      </c>
-      <c r="F1133" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1133" s="5"/>
+    </row>
+    <row r="1134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1134" s="6"/>
-      <c r="D1134" s="5" t="s">
-        <v>2873</v>
-      </c>
-      <c r="F1134" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1134" s="5"/>
+    </row>
+    <row r="1135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1135" s="6"/>
-      <c r="D1135" s="5" t="s">
-        <v>2874</v>
-      </c>
-      <c r="F1135" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1135" s="5"/>
+    </row>
+    <row r="1136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1136" s="6"/>
-      <c r="D1136" s="5" t="s">
-        <v>2875</v>
-      </c>
-      <c r="F1136" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1137" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1136" s="5"/>
+    </row>
+    <row r="1137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1137" s="6"/>
-      <c r="D1137" s="5" t="s">
-        <v>2876</v>
-      </c>
-      <c r="F1137" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1138" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1137" s="5"/>
+    </row>
+    <row r="1138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1138" s="6"/>
-      <c r="D1138" s="5" t="s">
-        <v>2877</v>
-      </c>
-      <c r="F1138" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1139" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1138" s="5"/>
+    </row>
+    <row r="1139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1139" s="6"/>
-      <c r="D1139" s="5" t="s">
-        <v>2878</v>
-      </c>
-      <c r="F1139" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1140" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1139" s="5"/>
+    </row>
+    <row r="1140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1140" s="6"/>
-      <c r="D1140" s="5" t="s">
-        <v>2879</v>
-      </c>
-      <c r="F1140" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1140" s="5"/>
+    </row>
+    <row r="1141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1141" s="6"/>
-      <c r="D1141" s="5" t="s">
-        <v>2880</v>
-      </c>
-      <c r="F1141" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1142" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1141" s="5"/>
+    </row>
+    <row r="1142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1142" s="6"/>
-      <c r="D1142" s="5" t="s">
-        <v>2881</v>
-      </c>
-      <c r="F1142" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1142" s="5"/>
+    </row>
+    <row r="1143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1143" s="6"/>
-      <c r="D1143" s="5" t="s">
-        <v>2882</v>
-      </c>
-      <c r="F1143" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1143" s="5"/>
+    </row>
+    <row r="1144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1144" s="6"/>
-      <c r="D1144" s="5" t="s">
-        <v>2883</v>
-      </c>
-      <c r="F1144" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1144" s="5"/>
+    </row>
+    <row r="1145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1145" s="6"/>
-      <c r="D1145" s="5" t="s">
-        <v>2884</v>
-      </c>
-      <c r="F1145" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1146" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1145" s="5"/>
+    </row>
+    <row r="1146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1146" s="6"/>
-      <c r="D1146" s="5" t="s">
-        <v>2885</v>
-      </c>
-      <c r="F1146" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1147" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1146" s="5"/>
+    </row>
+    <row r="1147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1147" s="6"/>
-      <c r="D1147" s="5" t="s">
-        <v>2886</v>
-      </c>
-      <c r="F1147" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1147" s="5"/>
+    </row>
+    <row r="1148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1148" s="6"/>
-      <c r="D1148" s="5" t="s">
-        <v>2887</v>
-      </c>
-      <c r="F1148" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1149" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1148" s="5"/>
+    </row>
+    <row r="1149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1149" s="6"/>
-      <c r="D1149" s="5" t="s">
-        <v>2888</v>
-      </c>
-      <c r="F1149" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1150" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="D1149" s="5"/>
+    </row>
+    <row r="1150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1150" s="6"/>
-      <c r="D1150" s="5" t="s">
-        <v>2889</v>
-      </c>
-      <c r="F1150" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1151" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1150" s="5"/>
+    </row>
+    <row r="1151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1151" s="6"/>
-      <c r="D1151" s="5" t="s">
-        <v>2890</v>
-      </c>
-      <c r="F1151" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1152" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1151" s="5"/>
+    </row>
+    <row r="1152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1152" s="6"/>
-      <c r="D1152" s="5" t="s">
-        <v>2891</v>
-      </c>
-      <c r="F1152" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1153" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1152" s="5"/>
+    </row>
+    <row r="1153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1153" s="6"/>
-      <c r="D1153" s="5" t="s">
-        <v>2892</v>
-      </c>
-      <c r="F1153" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1154" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1153" s="5"/>
+    </row>
+    <row r="1154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1154" s="6"/>
-      <c r="D1154" s="5" t="s">
-        <v>2893</v>
-      </c>
-      <c r="F1154" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1155" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1154" s="5"/>
+    </row>
+    <row r="1155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1155" s="6"/>
-      <c r="D1155" s="5" t="s">
-        <v>2894</v>
-      </c>
-      <c r="F1155" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1155" s="5"/>
+    </row>
+    <row r="1156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1156" s="6"/>
-      <c r="D1156" s="5" t="s">
-        <v>2895</v>
-      </c>
-      <c r="F1156" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1157" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1156" s="5"/>
+    </row>
+    <row r="1157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1157" s="6"/>
-      <c r="D1157" s="5" t="s">
-        <v>2896</v>
-      </c>
-      <c r="F1157" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1157" s="5"/>
+    </row>
+    <row r="1158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1158" s="6"/>
-      <c r="D1158" s="5" t="s">
-        <v>2897</v>
-      </c>
-      <c r="F1158" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1158" s="5"/>
+    </row>
+    <row r="1159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1159" s="6"/>
-      <c r="D1159" s="5" t="s">
-        <v>2898</v>
-      </c>
-      <c r="F1159" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1159" s="5"/>
+    </row>
+    <row r="1160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1160" s="6"/>
-      <c r="D1160" s="5" t="s">
-        <v>2899</v>
-      </c>
-      <c r="F1160" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1161" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1160" s="5"/>
+    </row>
+    <row r="1161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1161" s="6"/>
-      <c r="D1161" s="5" t="s">
-        <v>2900</v>
-      </c>
-      <c r="F1161" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1161" s="5"/>
+    </row>
+    <row r="1162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1162" s="6"/>
-      <c r="D1162" s="5" t="s">
-        <v>2901</v>
-      </c>
-      <c r="F1162" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1163" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1162" s="5"/>
+    </row>
+    <row r="1163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1163" s="6"/>
-      <c r="D1163" s="5" t="s">
-        <v>2902</v>
-      </c>
-      <c r="F1163" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1163" s="5"/>
+    </row>
+    <row r="1164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1164" s="6"/>
-      <c r="D1164" s="5" t="s">
-        <v>2903</v>
-      </c>
-      <c r="F1164" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1164" s="5"/>
+    </row>
+    <row r="1165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1165" s="6"/>
-      <c r="D1165" s="5" t="s">
-        <v>2904</v>
-      </c>
-      <c r="F1165" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1166" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1165" s="5"/>
+    </row>
+    <row r="1166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1166" s="6"/>
-      <c r="D1166" s="5" t="s">
-        <v>2905</v>
-      </c>
-      <c r="F1166" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1166" s="5"/>
+    </row>
+    <row r="1167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1167" s="6"/>
-      <c r="D1167" s="5" t="s">
-        <v>2906</v>
-      </c>
-      <c r="F1167" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1167" s="5"/>
+    </row>
+    <row r="1168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1168" s="6"/>
-      <c r="D1168" s="5" t="s">
-        <v>2907</v>
-      </c>
-      <c r="F1168" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1169" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1168" s="5"/>
+    </row>
+    <row r="1169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1169" s="6"/>
-      <c r="D1169" s="5" t="s">
-        <v>2908</v>
-      </c>
-      <c r="F1169" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1169" s="5"/>
+    </row>
+    <row r="1170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1170" s="6"/>
-      <c r="D1170" s="5" t="s">
-        <v>2909</v>
-      </c>
-      <c r="F1170" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1171" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1170" s="5"/>
+    </row>
+    <row r="1171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1171" s="6"/>
-      <c r="D1171" s="5" t="s">
-        <v>2910</v>
-      </c>
-      <c r="F1171" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1172" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1171" s="5"/>
+    </row>
+    <row r="1172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1172" s="6"/>
-      <c r="D1172" s="5" t="s">
-        <v>2911</v>
-      </c>
-      <c r="F1172" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1173" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1172" s="5"/>
+    </row>
+    <row r="1173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1173" s="6"/>
-      <c r="D1173" s="5" t="s">
-        <v>2912</v>
-      </c>
-      <c r="F1173" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1174" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D1173" s="5"/>
+    </row>
+    <row r="1174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1174" s="6"/>
-      <c r="D1174" s="5" t="s">
-        <v>2913</v>
-      </c>
-      <c r="F1174" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1175" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1174" s="5"/>
+    </row>
+    <row r="1175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1175" s="6"/>
-      <c r="D1175" s="5" t="s">
-        <v>2914</v>
-      </c>
-      <c r="F1175" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1176" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1175" s="5"/>
+    </row>
+    <row r="1176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1176" s="6"/>
-      <c r="D1176" s="5" t="s">
-        <v>2915</v>
-      </c>
-      <c r="F1176" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1176" s="5"/>
+    </row>
+    <row r="1177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1177" s="6"/>
-      <c r="D1177" s="5" t="s">
-        <v>2916</v>
-      </c>
-      <c r="F1177" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1178" spans="1:6" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="D1177" s="5"/>
+    </row>
+    <row r="1178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1178" s="6"/>
-      <c r="D1178" s="5" t="s">
-        <v>2917</v>
-      </c>
-      <c r="F1178" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1178" s="5"/>
+    </row>
+    <row r="1179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1179" s="6"/>
-      <c r="D1179" s="5" t="s">
-        <v>2918</v>
-      </c>
-      <c r="F1179" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1180" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1179" s="5"/>
+    </row>
+    <row r="1180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1180" s="6"/>
-      <c r="D1180" s="5" t="s">
-        <v>2919</v>
-      </c>
-      <c r="F1180" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1181" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1180" s="5"/>
+    </row>
+    <row r="1181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1181" s="6"/>
-      <c r="D1181" s="5" t="s">
-        <v>2920</v>
-      </c>
-      <c r="F1181" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1181" s="5"/>
+    </row>
+    <row r="1182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1182" s="6"/>
-      <c r="D1182" s="5" t="s">
-        <v>2921</v>
-      </c>
-      <c r="F1182" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1183" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1182" s="5"/>
+    </row>
+    <row r="1183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1183" s="6"/>
-      <c r="D1183" s="5" t="s">
-        <v>2922</v>
-      </c>
-      <c r="F1183" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1183" s="5"/>
+    </row>
+    <row r="1184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1184" s="6"/>
-      <c r="D1184" s="5" t="s">
-        <v>2923</v>
-      </c>
-      <c r="F1184" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1184" s="5"/>
+    </row>
+    <row r="1185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1185" s="6"/>
-      <c r="D1185" s="5" t="s">
-        <v>2924</v>
-      </c>
-      <c r="F1185" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1185" s="5"/>
+    </row>
+    <row r="1186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1186" s="6"/>
-      <c r="D1186" s="5" t="s">
-        <v>2925</v>
-      </c>
-      <c r="F1186" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1187" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1186" s="5"/>
+    </row>
+    <row r="1187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1187" s="6"/>
-      <c r="D1187" s="5" t="s">
-        <v>2926</v>
-      </c>
-      <c r="F1187" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1188" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1187" s="5"/>
+    </row>
+    <row r="1188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1188" s="6"/>
-      <c r="D1188" s="5" t="s">
-        <v>2927</v>
-      </c>
-      <c r="F1188" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1189" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1188" s="5"/>
+    </row>
+    <row r="1189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1189" s="6"/>
-      <c r="D1189" s="5" t="s">
-        <v>2926</v>
-      </c>
-      <c r="F1189" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1189" s="5"/>
+    </row>
+    <row r="1190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1190" s="6"/>
-      <c r="D1190" s="5" t="s">
-        <v>2928</v>
-      </c>
-      <c r="F1190" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1191" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1190" s="5"/>
+    </row>
+    <row r="1191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1191" s="6"/>
-      <c r="D1191" s="5" t="s">
-        <v>2926</v>
-      </c>
-      <c r="F1191" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1192" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="D1191" s="5"/>
+    </row>
+    <row r="1192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1192" s="6"/>
-      <c r="D1192" s="5" t="s">
-        <v>2929</v>
-      </c>
-      <c r="F1192" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1192" s="5"/>
+    </row>
+    <row r="1193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1193" s="6"/>
-      <c r="D1193" s="5" t="s">
-        <v>2930</v>
-      </c>
-      <c r="F1193" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1194" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1193" s="5"/>
+    </row>
+    <row r="1194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1194" s="6"/>
-      <c r="D1194" s="5" t="s">
-        <v>2931</v>
-      </c>
-      <c r="F1194" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1194" s="5"/>
+    </row>
+    <row r="1195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1195" s="6"/>
-      <c r="D1195" s="5" t="s">
-        <v>2932</v>
-      </c>
-      <c r="F1195" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1195" s="5"/>
+    </row>
+    <row r="1196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1196" s="6"/>
-      <c r="D1196" s="5" t="s">
-        <v>2933</v>
-      </c>
-      <c r="F1196" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1196" s="5"/>
+    </row>
+    <row r="1197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1197" s="6"/>
-      <c r="D1197" s="5" t="s">
-        <v>2934</v>
-      </c>
-      <c r="F1197" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1198" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D1197" s="5"/>
+    </row>
+    <row r="1198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1198" s="6"/>
-      <c r="D1198" s="5" t="s">
-        <v>2935</v>
-      </c>
-      <c r="F1198" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1198" s="5"/>
+    </row>
+    <row r="1199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1199" s="6"/>
-      <c r="D1199" s="5" t="s">
-        <v>2936</v>
-      </c>
-      <c r="F1199" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1200" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1199" s="5"/>
+    </row>
+    <row r="1200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1200" s="6"/>
-      <c r="D1200" s="5" t="s">
-        <v>2937</v>
-      </c>
-      <c r="F1200" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1201" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1200" s="5"/>
+    </row>
+    <row r="1201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1201" s="6"/>
-      <c r="D1201" s="5" t="s">
-        <v>2938</v>
-      </c>
-      <c r="F1201" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1201" s="5"/>
+    </row>
+    <row r="1202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1202" s="6"/>
-      <c r="D1202" s="5" t="s">
-        <v>2939</v>
-      </c>
-      <c r="F1202" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1202" s="5"/>
+    </row>
+    <row r="1203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1203" s="6"/>
-      <c r="D1203" s="5" t="s">
-        <v>2940</v>
-      </c>
-      <c r="F1203" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1204" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1203" s="5"/>
+    </row>
+    <row r="1204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1204" s="6"/>
-      <c r="D1204" s="5" t="s">
-        <v>2941</v>
-      </c>
-      <c r="F1204" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1205" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1204" s="5"/>
+    </row>
+    <row r="1205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1205" s="6"/>
-      <c r="D1205" s="5" t="s">
-        <v>2942</v>
-      </c>
-      <c r="F1205" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1205" s="5"/>
+    </row>
+    <row r="1206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1206" s="6"/>
-      <c r="D1206" s="5" t="s">
-        <v>2943</v>
-      </c>
-      <c r="F1206" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1207" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1206" s="5"/>
+    </row>
+    <row r="1207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1207" s="6"/>
-      <c r="D1207" s="5" t="s">
-        <v>2944</v>
-      </c>
-      <c r="F1207" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1208" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1207" s="5"/>
+    </row>
+    <row r="1208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1208" s="6"/>
-      <c r="D1208" s="5" t="s">
-        <v>2945</v>
-      </c>
-      <c r="F1208" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1208" s="5"/>
+    </row>
+    <row r="1209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1209" s="6"/>
-      <c r="D1209" s="5" t="s">
-        <v>2946</v>
-      </c>
-      <c r="F1209" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1209" s="5"/>
+    </row>
+    <row r="1210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1210" s="6"/>
-      <c r="D1210" s="5" t="s">
-        <v>2947</v>
-      </c>
-      <c r="F1210" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1210" s="5"/>
+    </row>
+    <row r="1211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1211" s="6"/>
-      <c r="D1211" s="5" t="s">
-        <v>2948</v>
-      </c>
-      <c r="F1211" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1211" s="5"/>
+    </row>
+    <row r="1212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1212" s="6"/>
-      <c r="D1212" s="5" t="s">
-        <v>2949</v>
-      </c>
-      <c r="F1212" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1212" s="5"/>
+    </row>
+    <row r="1213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1213" s="6"/>
-      <c r="D1213" s="5" t="s">
-        <v>2950</v>
-      </c>
-      <c r="F1213" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1213" s="5"/>
+    </row>
+    <row r="1214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1214" s="6"/>
-      <c r="D1214" s="5" t="s">
-        <v>2951</v>
-      </c>
-      <c r="F1214" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1215" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1214" s="5"/>
+    </row>
+    <row r="1215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1215" s="6"/>
-      <c r="D1215" s="5" t="s">
-        <v>2952</v>
-      </c>
-      <c r="F1215" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1215" s="5"/>
+    </row>
+    <row r="1216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1216" s="6"/>
-      <c r="D1216" s="5" t="s">
-        <v>2953</v>
-      </c>
-      <c r="F1216" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1216" s="5"/>
     </row>
     <row r="1217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1217" s="6"/>
-      <c r="D1217" s="5" t="s">
-        <v>2954</v>
-      </c>
-      <c r="F1217" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1217" s="5"/>
     </row>
     <row r="1218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1218" s="6"/>
-      <c r="D1218" s="5" t="s">
-        <v>2955</v>
-      </c>
-      <c r="F1218" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1218" s="5"/>
     </row>
     <row r="1219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1219" s="6"/>
-      <c r="D1219" s="5" t="s">
-        <v>2956</v>
-      </c>
-      <c r="F1219" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1219" s="5"/>
     </row>
     <row r="1220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1220" s="6"/>
-      <c r="D1220" t="s">
-        <v>2957</v>
-      </c>
-      <c r="F1220" t="s">
-        <v>1878</v>
-      </c>
     </row>
     <row r="1221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1221" s="6"/>
-      <c r="D1221" s="4" t="s">
-        <v>2959</v>
-      </c>
-      <c r="F1221" s="2" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1221" s="4"/>
+      <c r="F1221" s="2"/>
     </row>
     <row r="1222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1222" s="6"/>
-      <c r="D1222" s="4" t="s">
-        <v>2960</v>
-      </c>
-      <c r="F1222" s="2" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1222" s="4"/>
+      <c r="F1222" s="2"/>
     </row>
     <row r="1223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1223" s="6"/>
-      <c r="D1223" s="4" t="s">
-        <v>2961</v>
-      </c>
-      <c r="F1223" s="2" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1223" s="4"/>
+      <c r="F1223" s="2"/>
     </row>
     <row r="1224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1224" s="6"/>
-      <c r="D1224" s="4" t="s">
-        <v>2962</v>
-      </c>
-      <c r="F1224" s="2" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1224" s="4"/>
+      <c r="F1224" s="2"/>
     </row>
     <row r="1225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1225" s="6"/>
-      <c r="D1225" s="4" t="s">
-        <v>2963</v>
-      </c>
-      <c r="F1225" s="2" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1225" s="4"/>
+      <c r="F1225" s="2"/>
     </row>
     <row r="1226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1226" s="6"/>
-      <c r="D1226" s="4" t="s">
-        <v>2964</v>
-      </c>
-      <c r="F1226" s="2" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1226" s="4"/>
+      <c r="F1226" s="2"/>
     </row>
     <row r="1227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1227" s="6"/>
-      <c r="D1227" s="4" t="s">
-        <v>2965</v>
-      </c>
-      <c r="F1227" s="2" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1227" s="4"/>
+      <c r="F1227" s="2"/>
     </row>
     <row r="1228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1228" s="6"/>
-      <c r="D1228" s="5" t="s">
-        <v>2966</v>
-      </c>
-      <c r="F1228" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1228" s="5"/>
     </row>
     <row r="1229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1229" s="6"/>
-      <c r="D1229" s="5" t="s">
-        <v>2967</v>
-      </c>
-      <c r="F1229" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1229" s="5"/>
     </row>
     <row r="1230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1230" s="6"/>
-      <c r="D1230" s="5" t="s">
-        <v>2968</v>
-      </c>
-      <c r="F1230" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1230" s="5"/>
     </row>
     <row r="1231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1231" s="6"/>
-      <c r="D1231" s="5" t="s">
-        <v>2969</v>
-      </c>
-      <c r="F1231" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1231" s="5"/>
     </row>
     <row r="1232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1232" s="6"/>
-      <c r="D1232" s="5" t="s">
-        <v>2970</v>
-      </c>
-      <c r="F1232" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1233" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1232" s="5"/>
+    </row>
+    <row r="1233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1233" s="6"/>
-      <c r="D1233" s="5" t="s">
-        <v>2971</v>
-      </c>
-      <c r="F1233" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1233" s="5"/>
+    </row>
+    <row r="1234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1234" s="6"/>
-      <c r="D1234" s="5" t="s">
-        <v>2972</v>
-      </c>
-      <c r="F1234" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1235" spans="1:6" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="D1234" s="5"/>
+    </row>
+    <row r="1235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1235" s="6"/>
-      <c r="D1235" s="5" t="s">
-        <v>2973</v>
-      </c>
-      <c r="F1235" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1235" s="5"/>
+    </row>
+    <row r="1236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1236" s="6"/>
-      <c r="D1236" s="5" t="s">
-        <v>2974</v>
-      </c>
-      <c r="F1236" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1237" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1236" s="5"/>
+    </row>
+    <row r="1237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1237" s="6"/>
-      <c r="D1237" s="5" t="s">
-        <v>2975</v>
-      </c>
-      <c r="F1237" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1238" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1237" s="5"/>
+    </row>
+    <row r="1238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1238" s="6"/>
-      <c r="D1238" s="5" t="s">
-        <v>2976</v>
-      </c>
-      <c r="F1238" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1238" s="5"/>
+    </row>
+    <row r="1239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1239" s="6"/>
-      <c r="D1239" s="5" t="s">
-        <v>2958</v>
-      </c>
-      <c r="F1239" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1239" s="5"/>
+    </row>
+    <row r="1240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1240" s="6"/>
-      <c r="D1240" s="5" t="s">
-        <v>2977</v>
-      </c>
-      <c r="F1240" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1240" s="5"/>
+    </row>
+    <row r="1241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1241" s="6"/>
-      <c r="D1241" s="5" t="s">
-        <v>2978</v>
-      </c>
-      <c r="F1241" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1241" s="5"/>
+    </row>
+    <row r="1242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1242" s="6"/>
-      <c r="D1242" s="5" t="s">
-        <v>2979</v>
-      </c>
-      <c r="F1242" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1242" s="5"/>
+    </row>
+    <row r="1243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1243" s="6"/>
-      <c r="D1243" s="5" t="s">
-        <v>2980</v>
-      </c>
-      <c r="F1243" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1243" s="5"/>
+    </row>
+    <row r="1244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1244" s="6"/>
-      <c r="D1244" s="5" t="s">
-        <v>2764</v>
-      </c>
-      <c r="F1244" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1244" s="5"/>
+    </row>
+    <row r="1245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1245" s="6"/>
-      <c r="D1245" t="s">
-        <v>2981</v>
-      </c>
-      <c r="F1245" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1246" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1246" s="6"/>
-      <c r="D1246" s="5" t="s">
-        <v>2839</v>
-      </c>
-      <c r="F1246" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1247" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1246" s="5"/>
+    </row>
+    <row r="1247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1247" s="6"/>
-      <c r="D1247" s="5" t="s">
-        <v>2982</v>
-      </c>
-      <c r="F1247" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1248" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1247" s="5"/>
+    </row>
+    <row r="1248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1248" s="6"/>
-      <c r="D1248" s="5" t="s">
-        <v>2983</v>
-      </c>
-      <c r="F1248" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1249" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="D1248" s="5"/>
+    </row>
+    <row r="1249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1249" s="6"/>
-      <c r="D1249" s="5" t="s">
-        <v>2984</v>
-      </c>
-      <c r="F1249" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1250" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1249" s="5"/>
+    </row>
+    <row r="1250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1250" s="6"/>
-      <c r="D1250" s="5" t="s">
-        <v>2985</v>
-      </c>
-      <c r="F1250" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1251" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1250" s="5"/>
+    </row>
+    <row r="1251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1251" s="6"/>
-      <c r="D1251" s="5" t="s">
-        <v>2986</v>
-      </c>
-      <c r="F1251" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1252" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1251" s="5"/>
+    </row>
+    <row r="1252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1252" s="6"/>
-      <c r="D1252" s="5" t="s">
-        <v>2987</v>
-      </c>
-      <c r="F1252" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1252" s="5"/>
+    </row>
+    <row r="1253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1253" s="6"/>
-      <c r="D1253" s="5" t="s">
-        <v>2988</v>
-      </c>
-      <c r="F1253" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1254" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1253" s="5"/>
+    </row>
+    <row r="1254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1254" s="6"/>
-      <c r="D1254" s="5" t="s">
-        <v>2989</v>
-      </c>
-      <c r="F1254" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1255" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1254" s="5"/>
+    </row>
+    <row r="1255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1255" s="6"/>
-      <c r="D1255" s="5" t="s">
-        <v>2990</v>
-      </c>
-      <c r="F1255" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1256" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1255" s="5"/>
+    </row>
+    <row r="1256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1256" s="6"/>
-      <c r="D1256" s="5" t="s">
-        <v>2991</v>
-      </c>
-      <c r="F1256" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1257" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1256" s="5"/>
+    </row>
+    <row r="1257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1257" s="6"/>
-      <c r="D1257" s="5" t="s">
-        <v>2992</v>
-      </c>
-      <c r="F1257" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1258" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="D1257" s="5"/>
+    </row>
+    <row r="1258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1258" s="6"/>
-      <c r="D1258" s="5" t="s">
-        <v>2993</v>
-      </c>
-      <c r="F1258" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1259" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1258" s="5"/>
+    </row>
+    <row r="1259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1259" s="6"/>
-      <c r="D1259" s="5" t="s">
-        <v>2994</v>
-      </c>
-      <c r="F1259" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1260" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="D1259" s="5"/>
+    </row>
+    <row r="1260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1260" s="6"/>
-      <c r="D1260" s="5" t="s">
-        <v>2995</v>
-      </c>
-      <c r="F1260" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1261" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="D1260" s="5"/>
+    </row>
+    <row r="1261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1261" s="6"/>
-      <c r="D1261" s="5" t="s">
-        <v>2996</v>
-      </c>
-      <c r="F1261" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1262" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1261" s="5"/>
+    </row>
+    <row r="1262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1262" s="6"/>
-      <c r="D1262" s="5" t="s">
-        <v>2856</v>
-      </c>
-      <c r="F1262" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1263" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1262" s="5"/>
+    </row>
+    <row r="1263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1263" s="6"/>
-      <c r="D1263" s="5" t="s">
-        <v>2997</v>
-      </c>
-      <c r="F1263" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1264" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="D1263" s="5"/>
+    </row>
+    <row r="1264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1264" s="6"/>
-      <c r="D1264" s="5" t="s">
-        <v>2998</v>
-      </c>
-      <c r="F1264" t="s">
-        <v>1877</v>
-      </c>
+      <c r="D1264" s="5"/>
     </row>
     <row r="1265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1265" s="6"/>
-      <c r="D1265" s="4" t="s">
-        <v>2999</v>
-      </c>
-      <c r="F1265" s="2" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1265" s="4"/>
+      <c r="F1265" s="2"/>
     </row>
     <row r="1266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1266" s="6"/>
-      <c r="D1266" s="5" t="s">
-        <v>3000</v>
-      </c>
-      <c r="F1266" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1267" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="D1266" s="5"/>
+    </row>
+    <row r="1267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1267" s="6"/>
-      <c r="D1267" s="5" t="s">
-        <v>3001</v>
-      </c>
-      <c r="F1267" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1267" s="5"/>
     </row>
     <row r="1268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1268" s="6"/>
-      <c r="D1268" s="5" t="s">
-        <v>3002</v>
-      </c>
-      <c r="F1268" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1268" s="5"/>
     </row>
     <row r="1269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1269" s="6"/>
-      <c r="D1269" s="5" t="s">
-        <v>3003</v>
-      </c>
-      <c r="F1269" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1269" s="5"/>
     </row>
     <row r="1270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1270" s="6"/>
-      <c r="D1270" s="5" t="s">
-        <v>3004</v>
-      </c>
-      <c r="F1270" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1270" s="5"/>
     </row>
     <row r="1271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1271" s="6"/>
-      <c r="D1271" s="5" t="s">
-        <v>3005</v>
-      </c>
-      <c r="F1271" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1271" s="5"/>
     </row>
     <row r="1272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1272" s="6"/>
-      <c r="D1272" s="5" t="s">
-        <v>3006</v>
-      </c>
-      <c r="F1272" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1272" s="5"/>
     </row>
     <row r="1273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1273" s="6"/>
-      <c r="D1273" s="5" t="s">
-        <v>3007</v>
-      </c>
-      <c r="F1273" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1273" s="5"/>
     </row>
     <row r="1274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1274" s="6"/>
-      <c r="D1274" s="5" t="s">
-        <v>3008</v>
-      </c>
-      <c r="F1274" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1274" s="5"/>
     </row>
     <row r="1275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1275" s="6"/>
-      <c r="D1275" s="5" t="s">
-        <v>3009</v>
-      </c>
-      <c r="F1275" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1275" s="5"/>
     </row>
     <row r="1276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1276" s="6"/>
-      <c r="D1276" s="5" t="s">
-        <v>3010</v>
-      </c>
-      <c r="F1276" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1276" s="5"/>
     </row>
     <row r="1277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1277" s="6"/>
-      <c r="D1277" s="5" t="s">
-        <v>3011</v>
-      </c>
-      <c r="F1277" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1277" s="5"/>
     </row>
     <row r="1278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1278" s="6"/>
-      <c r="D1278" s="5" t="s">
-        <v>3012</v>
-      </c>
-      <c r="F1278" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1278" s="5"/>
     </row>
     <row r="1279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1279" s="6"/>
-      <c r="D1279" s="5" t="s">
-        <v>3013</v>
-      </c>
-      <c r="F1279" t="s">
-        <v>1878</v>
-      </c>
+      <c r="D1279" s="5"/>
     </row>
     <row r="1280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1280" s="6"/>
-      <c r="D1280" s="5" t="s">
-        <v>3014</v>
-      </c>
-      <c r="F1280" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1281" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1280" s="5"/>
+    </row>
+    <row r="1281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1281" s="6"/>
-      <c r="D1281" s="5" t="s">
-        <v>3015</v>
-      </c>
-      <c r="F1281" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1282" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D1281" s="5"/>
+    </row>
+    <row r="1282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1282" s="6"/>
-      <c r="D1282" s="5" t="s">
-        <v>3016</v>
-      </c>
-      <c r="F1282" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1283" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1282" s="5"/>
+    </row>
+    <row r="1283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1283" s="6"/>
-      <c r="D1283" s="5" t="s">
-        <v>3017</v>
-      </c>
-      <c r="F1283" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1284" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1283" s="5"/>
+    </row>
+    <row r="1284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1284" s="6"/>
-      <c r="D1284" s="5" t="s">
-        <v>3018</v>
-      </c>
-      <c r="F1284" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1284" s="5"/>
+    </row>
+    <row r="1285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1285" s="6"/>
-      <c r="D1285" s="5" t="s">
-        <v>3019</v>
-      </c>
-      <c r="F1285" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1285" s="5"/>
+    </row>
+    <row r="1286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1286" s="6"/>
-      <c r="D1286" s="5" t="s">
-        <v>3020</v>
-      </c>
-      <c r="F1286" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1287" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1286" s="5"/>
+    </row>
+    <row r="1287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1287" s="6"/>
-      <c r="D1287" s="5" t="s">
-        <v>3021</v>
-      </c>
-      <c r="F1287" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1287" s="5"/>
+    </row>
+    <row r="1288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1288" s="6"/>
-      <c r="D1288" s="5" t="s">
-        <v>3022</v>
-      </c>
-      <c r="F1288" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1288" s="5"/>
+    </row>
+    <row r="1289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1289" s="6"/>
-      <c r="D1289" s="5" t="s">
-        <v>3007</v>
-      </c>
-      <c r="F1289" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1289" s="5"/>
+    </row>
+    <row r="1290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1290" s="6"/>
-      <c r="D1290" s="5" t="s">
-        <v>3008</v>
-      </c>
-      <c r="F1290" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1290" s="5"/>
+    </row>
+    <row r="1291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1291" s="6"/>
-      <c r="D1291" s="5" t="s">
-        <v>3003</v>
-      </c>
-      <c r="F1291" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1291" s="5"/>
+    </row>
+    <row r="1292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1292" s="6"/>
-      <c r="D1292" s="5" t="s">
-        <v>3023</v>
-      </c>
-      <c r="F1292" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1292" s="5"/>
+    </row>
+    <row r="1293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1293" s="6"/>
-      <c r="D1293" s="5" t="s">
-        <v>3024</v>
-      </c>
-      <c r="F1293" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1293" s="5"/>
+    </row>
+    <row r="1294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1294" s="6"/>
-      <c r="D1294" s="5" t="s">
-        <v>3025</v>
-      </c>
-      <c r="F1294" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1295" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D1294" s="5"/>
+    </row>
+    <row r="1295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1295" s="6"/>
-      <c r="D1295" s="5" t="s">
-        <v>3026</v>
-      </c>
-      <c r="F1295" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1295" s="5"/>
+    </row>
+    <row r="1296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1296" s="6"/>
-      <c r="D1296" s="5" t="s">
-        <v>3027</v>
-      </c>
-      <c r="F1296" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1297" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1296" s="5"/>
+    </row>
+    <row r="1297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1297" s="6"/>
-      <c r="D1297" s="5" t="s">
-        <v>3028</v>
-      </c>
-      <c r="F1297" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1298" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D1297" s="5"/>
+    </row>
+    <row r="1298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1298" s="6"/>
-      <c r="D1298" s="5" t="s">
-        <v>3029</v>
-      </c>
-      <c r="F1298" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1299" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1298" s="5"/>
+    </row>
+    <row r="1299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1299" s="6"/>
-      <c r="D1299" s="5" t="s">
-        <v>3030</v>
-      </c>
-      <c r="F1299" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1300" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1299" s="5"/>
+    </row>
+    <row r="1300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1300" s="6"/>
-      <c r="D1300" s="5" t="s">
-        <v>3031</v>
-      </c>
-      <c r="F1300" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1301" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1300" s="5"/>
+    </row>
+    <row r="1301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1301" s="6"/>
-      <c r="D1301" s="5" t="s">
-        <v>3032</v>
-      </c>
-      <c r="F1301" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="1302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1301" s="5"/>
+    </row>
+    <row r="1302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1302" s="6"/>
       <c r="D1302" s="5"/>
     </row>
-    <row r="1303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1303" s="6"/>
       <c r="D1303" s="5"/>
     </row>
-    <row r="1304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1304" s="6"/>
       <c r="D1304" s="5"/>
     </row>
-    <row r="1305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1305" s="6"/>
       <c r="D1305" s="5"/>
     </row>
-    <row r="1306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1306" s="6"/>
       <c r="D1306" s="5"/>
     </row>
-    <row r="1307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1307" s="6"/>
       <c r="D1307" s="5"/>
     </row>
-    <row r="1308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1308" s="6"/>
       <c r="D1308" s="5"/>
     </row>
-    <row r="1309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1309" s="6"/>
       <c r="D1309" s="5"/>
     </row>
-    <row r="1310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1310" s="6"/>
       <c r="D1310" s="5"/>
     </row>
-    <row r="1311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1311" s="6"/>
       <c r="D1311" s="5"/>
     </row>
-    <row r="1312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1312" s="6"/>
       <c r="D1312" s="5"/>
     </row>

</xml_diff>